<commit_message>
DAO implemented and BugLocator's elapsed time measured. Release for v0.6
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaus\Dropbox\Workspace\BLIA\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="25215" windowHeight="14535"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="25220" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="DB schema design" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="127">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -102,6 +97,10 @@
   </si>
   <si>
     <t>BL_SCORE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHECKIN_DATE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -500,7 +499,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -537,16 +536,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>COMM_DATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source file &amp; version ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Fixed function ID</t>
+  </si>
+  <si>
+    <t>Fixed source file ID</t>
   </si>
 </sst>
 </file>
@@ -557,7 +550,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -565,14 +558,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -581,7 +574,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -590,7 +583,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -598,7 +591,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -610,9 +603,10 @@
       <charset val="129"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -660,7 +654,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -680,6 +674,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -725,18 +737,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle name="보통" xfId="1" builtinId="28"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="좋음" xfId="6" builtinId="26"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1006,7 +1024,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1016,1045 +1034,1032 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.125" customWidth="1"/>
-    <col min="5" max="5" width="21.125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="31.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.625" customWidth="1"/>
-    <col min="9" max="9" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28">
+      <c r="A4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28">
       <c r="A9" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="K16" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="C19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="E19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="I29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:11" ht="15">
       <c r="A31" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="28">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="E38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J35" s="3" t="s">
+      <c r="G38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15">
+      <c r="A39" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K35" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I36" s="1" t="s">
+      <c r="C40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I38" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="J40" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="I44" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I44" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:11" ht="15">
       <c r="A45" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="51" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C61" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
DB module of BugRepoAnalyzer implemented & tested complete.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="157">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -597,10 +597,6 @@
   </si>
   <si>
     <t>IDX_COMM_FILE_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_INT_ANALYSIS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -685,6 +681,15 @@
   </si>
   <si>
     <t>Bug와 Source File의 corpus 간의 분석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_INT_ANAL_BUG_ID,
+UNIQUE COMP_IDX_INT_ANALSYS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_INT_ANALSYS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -773,7 +778,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -799,6 +804,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -865,7 +876,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -906,6 +917,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="12" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1202,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1219,7 +1233,7 @@
     <col min="9" max="9" width="5.625" customWidth="1"/>
     <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1663,7 +1677,7 @@
         <v>100</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
@@ -1696,7 +1710,7 @@
         <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>71</v>
@@ -1720,7 +1734,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
@@ -1760,7 +1774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>20</v>
       </c>
@@ -1768,7 +1782,7 @@
         <v>99</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>35</v>
@@ -1788,8 +1802,8 @@
       <c r="K24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>140</v>
+      <c r="L24" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>56</v>
@@ -1803,7 +1817,7 @@
         <v>99</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -1817,13 +1831,15 @@
       <c r="H25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="14" t="s">
         <v>123</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L25" s="1"/>
+      <c r="L25" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="M25" s="1" t="s">
         <v>124</v>
       </c>
@@ -2143,7 +2159,7 @@
         <v>101</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>71</v>
@@ -2160,7 +2176,7 @@
         <v>101</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M41" s="1" t="s">
         <v>96</v>
@@ -2220,7 +2236,7 @@
         <v>100</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>60</v>
@@ -2228,13 +2244,13 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>71</v>
@@ -2242,10 +2258,10 @@
     </row>
     <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -2268,7 +2284,7 @@
         <v>101</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>56</v>
@@ -2276,13 +2292,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>40</v>
@@ -2348,10 +2364,10 @@
     </row>
     <row r="57" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" t="s">
         <v>151</v>
-      </c>
-      <c r="B57" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2374,7 +2390,7 @@
         <v>101</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>56</v>
@@ -2388,7 +2404,7 @@
         <v>99</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
All DB modules were linked to BugLocator and implemented/tested.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1216,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
TopN, MRR were implemented and it's testing was done.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1216,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1225,7 +1225,7 @@
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="6.125" customWidth="1"/>
     <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="17.125" hidden="1" customWidth="1"/>

</xml_diff>

<commit_message>
All failed testcases were fixed. Full tests were passed.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaus\Dropbox\Workspace\BLIA\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="8580" windowHeight="7485"/>
+    <workbookView xWindow="-1680" yWindow="-17980" windowWidth="27940" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="DB schema design" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -492,7 +487,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -659,7 +654,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -670,7 +665,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -701,7 +696,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -709,14 +704,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -725,7 +720,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -734,7 +729,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -742,7 +737,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -756,7 +751,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -764,7 +759,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -772,7 +767,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -924,19 +919,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="40% - 강조색2" xfId="12" builtinId="35"/>
-    <cellStyle name="강조색2" xfId="11" builtinId="33"/>
-    <cellStyle name="보통" xfId="1" builtinId="28"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="좋음" xfId="6" builtinId="26"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="40% - Accent2" xfId="12" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="11" builtinId="33"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1206,7 +1201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1216,28 +1211,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1"/>
-    <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" customWidth="1"/>
-    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
@@ -1248,7 +1243,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="28">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1318,7 +1313,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="28">
       <c r="A4" s="11" t="s">
         <v>115</v>
       </c>
@@ -1353,7 +1348,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="11" t="s">
         <v>72</v>
       </c>
@@ -1386,7 +1381,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="J6" s="1" t="s">
         <v>88</v>
       </c>
@@ -1398,7 +1393,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1406,7 +1401,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1430,7 +1425,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" s="10" t="s">
         <v>104</v>
       </c>
@@ -1461,7 +1456,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="28">
       <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
@@ -1496,7 +1491,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" s="11" t="s">
         <v>105</v>
       </c>
@@ -1529,7 +1524,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>113</v>
       </c>
@@ -1550,7 +1545,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
         <v>126</v>
       </c>
@@ -1571,7 +1566,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1592,7 +1587,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15">
       <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
@@ -1603,7 +1598,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1634,7 +1629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18" s="10" t="s">
         <v>10</v>
       </c>
@@ -1669,7 +1664,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19" s="12" t="s">
         <v>108</v>
       </c>
@@ -1702,7 +1697,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="A20" s="11" t="s">
         <v>72</v>
       </c>
@@ -1729,7 +1724,7 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="22" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15">
       <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1774,7 +1769,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="28">
       <c r="A24" s="11" t="s">
         <v>20</v>
       </c>
@@ -1809,7 +1804,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="11" t="s">
         <v>13</v>
       </c>
@@ -1844,7 +1839,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1875,7 +1870,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1906,7 +1901,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1937,7 +1932,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1968,7 +1963,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>107</v>
       </c>
@@ -1995,12 +1990,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="15">
       <c r="A32" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15">
       <c r="A33" s="3" t="s">
         <v>27</v>
       </c>
@@ -2015,7 +2010,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="28">
       <c r="A34" s="10" t="s">
         <v>8</v>
       </c>
@@ -2039,7 +2034,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13">
       <c r="A35" s="11" t="s">
         <v>72</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -2085,7 +2080,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>118</v>
       </c>
@@ -2107,7 +2102,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13">
       <c r="A38" s="4" t="s">
         <v>126</v>
       </c>
@@ -2129,7 +2124,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>119</v>
       </c>
@@ -2151,7 +2146,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13">
       <c r="J40" s="11" t="s">
         <v>72</v>
       </c>
@@ -2165,7 +2160,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="15">
       <c r="A41" s="6" t="s">
         <v>59</v>
       </c>
@@ -2182,7 +2177,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13">
       <c r="A42" s="3" t="s">
         <v>27</v>
       </c>
@@ -2204,7 +2199,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13">
       <c r="A43" s="10" t="s">
         <v>11</v>
       </c>
@@ -2228,7 +2223,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13">
       <c r="A44" s="11" t="s">
         <v>108</v>
       </c>
@@ -2242,7 +2237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13">
       <c r="A45" s="13" t="s">
         <v>142</v>
       </c>
@@ -2256,7 +2251,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="15">
       <c r="A47" s="6" t="s">
         <v>149</v>
       </c>
@@ -2264,7 +2259,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13">
       <c r="A48" s="3" t="s">
         <v>27</v>
       </c>
@@ -2276,7 +2271,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" s="11" t="s">
         <v>6</v>
       </c>
@@ -2290,7 +2285,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" s="13" t="s">
         <v>153</v>
       </c>
@@ -2304,7 +2299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -2316,7 +2311,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -2328,7 +2323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
@@ -2340,7 +2335,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -2352,7 +2347,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
@@ -2362,7 +2357,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="57" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15">
       <c r="A57" s="6" t="s">
         <v>150</v>
       </c>
@@ -2370,7 +2365,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
         <v>27</v>
       </c>
@@ -2382,7 +2377,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
@@ -2396,7 +2391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
         <v>12</v>
       </c>
@@ -2410,7 +2405,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -2420,12 +2415,12 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="63" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15">
       <c r="A63" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" s="3" t="s">
         <v>27</v>
       </c>
@@ -2437,7 +2432,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" s="11" t="s">
         <v>6</v>
       </c>
@@ -2451,7 +2446,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66" s="8" t="s">
         <v>120</v>
       </c>
@@ -2463,7 +2458,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4">
       <c r="A67" s="9" t="s">
         <v>121</v>
       </c>
@@ -2475,12 +2470,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15">
       <c r="A69" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
         <v>27</v>
       </c>
@@ -2492,7 +2487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" s="12" t="s">
         <v>134</v>
       </c>
@@ -2506,7 +2501,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -2518,7 +2513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
         <v>16</v>
       </c>
@@ -2531,7 +2526,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Implemented stack-trace extraction & imported classes info modules
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaus\Dropbox\Workspace\BLIA\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1680" yWindow="-17980" windowWidth="27940" windowHeight="17460"/>
+    <workbookView xWindow="-1680" yWindow="-17985" windowWidth="27945" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="DB schema design" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="163">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -258,10 +263,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Stacktace set</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>BUG_COR_INFO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -437,10 +438,6 @@
   </si>
   <si>
     <t>VARCHAR(15)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(2047)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -487,7 +484,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -509,10 +506,6 @@
   </si>
   <si>
     <t>COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>STRACE_SET</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -654,7 +647,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -665,7 +658,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -687,16 +680,52 @@
     <t>UNIQUE COMP_IDX_INT_ANALSYS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>BUG_ID(KEY)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_STRACE_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imported class in the source file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_IMP_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMP_CLASS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_SF_IMP_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_STRACE_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>STRACE_CLASS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class in stack-trace from bug report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -704,14 +733,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -720,7 +749,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -729,7 +758,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -737,7 +766,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -751,7 +780,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -759,7 +788,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -767,7 +796,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -871,7 +907,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -917,21 +953,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="40% - Accent2" xfId="12" builtinId="35"/>
-    <cellStyle name="Accent2" xfId="11" builtinId="33"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - 강조색2" xfId="12" builtinId="35"/>
+    <cellStyle name="강조색2" xfId="11" builtinId="33"/>
+    <cellStyle name="보통" xfId="1" builtinId="28"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="좋음" xfId="6" builtinId="26"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1201,7 +1243,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1209,30 +1251,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.125" customWidth="1"/>
+    <col min="5" max="5" width="6.125" customWidth="1"/>
+    <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.625" customWidth="1"/>
+    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15">
+    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
@@ -1240,10 +1280,10 @@
         <v>51</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1251,7 +1291,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>29</v>
@@ -1272,21 +1312,21 @@
         <v>28</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28">
+    <row r="3" spans="1:13" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -1295,33 +1335,33 @@
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="28">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>33</v>
@@ -1330,70 +1370,70 @@
         <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1401,7 +1441,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15">
+    <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1422,25 +1462,25 @@
         <v>29</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>49</v>
@@ -1456,15 +1496,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28">
+    <row r="10" spans="1:13" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>31</v>
@@ -1473,42 +1513,42 @@
         <v>19</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>36</v>
@@ -1517,61 +1557,61 @@
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="1" t="s">
@@ -1581,13 +1621,13 @@
         <v>1</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15">
+    <row r="16" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
@@ -1595,10 +1635,10 @@
         <v>53</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1629,15 +1669,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -1646,99 +1686,96 @@
         <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J18" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="12" t="s">
-        <v>108</v>
-      </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>50</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="22" spans="1:13" ht="15">
+    <row r="22" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1769,24 +1806,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="28">
-      <c r="A24" s="11" t="s">
-        <v>20</v>
+    <row r="24" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>49</v>
@@ -1795,66 +1832,54 @@
         <v>6</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="11" t="s">
-        <v>13</v>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>158</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>144</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>43</v>
@@ -1863,29 +1888,25 @@
         <v>15</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>149</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>44</v>
@@ -1894,29 +1915,29 @@
         <v>14</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>45</v>
@@ -1925,103 +1946,126 @@
         <v>18</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="4"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="D29" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F30" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H30" s="1"/>
       <c r="J30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15">
-      <c r="A32" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="15">
-      <c r="A33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>29</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="28">
-      <c r="A34" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>27</v>
@@ -2034,338 +2078,304 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>71</v>
-      </c>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>37</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
-        <v>128</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="1" t="s">
-        <v>119</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1" t="s">
-        <v>58</v>
+        <v>100</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M41" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
-      <c r="J40" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="15">
-      <c r="A41" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J41" s="11" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="K42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B44" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="15">
-      <c r="A47" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A54" s="16" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="B54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="57" spans="1:4" ht="15">
+      <c r="C55" s="4"/>
+      <c r="D55" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>27</v>
       </c>
@@ -2377,156 +2387,262 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="11" t="s">
-        <v>12</v>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-    </row>
-    <row r="63" spans="1:4" ht="15">
-      <c r="A63" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="3" t="s">
+      <c r="D61" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="4"/>
+      <c r="D63" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="4"/>
+      <c r="D64" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="67" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="11" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D65" s="1" t="s">
+      <c r="B69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+    </row>
+    <row r="73" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A73" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15">
-      <c r="A69" s="6" t="s">
+    <row r="79" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="1" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="B83" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
StackTraceAnalyzer implemented and tested.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaus\Dropbox\Workspace\BLIA\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1680" yWindow="-17985" windowWidth="27945" windowHeight="17460"/>
+    <workbookView xWindow="140" yWindow="80" windowWidth="27940" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="DB schema design" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="164">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -484,7 +479,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -647,7 +642,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -658,7 +653,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -715,6 +710,9 @@
   <si>
     <t>Class in stack-trace from bug report</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VER</t>
   </si>
 </sst>
 </file>
@@ -725,7 +723,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -733,14 +731,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -749,7 +747,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -758,7 +756,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -766,7 +764,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -780,7 +778,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -788,7 +786,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -796,14 +794,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -868,7 +866,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -904,6 +902,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -960,20 +964,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
-    <cellStyle name="40% - 강조색2" xfId="12" builtinId="35"/>
-    <cellStyle name="강조색2" xfId="11" builtinId="33"/>
-    <cellStyle name="보통" xfId="1" builtinId="28"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="좋음" xfId="6" builtinId="26"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
+  <cellStyles count="15">
+    <cellStyle name="40% - Accent2" xfId="12" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="11" builtinId="33"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1243,7 +1249,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1253,26 +1259,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.125" customWidth="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1"/>
-    <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" customWidth="1"/>
-    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
@@ -1283,7 +1291,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="28">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1353,7 +1361,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="28">
       <c r="A4" s="11" t="s">
         <v>113</v>
       </c>
@@ -1388,7 +1396,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -1421,7 +1429,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="J6" s="1" t="s">
         <v>87</v>
       </c>
@@ -1433,7 +1441,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1441,7 +1449,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1465,7 +1473,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" s="10" t="s">
         <v>102</v>
       </c>
@@ -1496,7 +1504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="28">
       <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1539,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" s="11" t="s">
         <v>103</v>
       </c>
@@ -1564,7 +1572,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>111</v>
       </c>
@@ -1585,7 +1593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
         <v>123</v>
       </c>
@@ -1606,7 +1614,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1627,7 +1635,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15">
       <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
@@ -1638,7 +1646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1669,7 +1677,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18" s="10" t="s">
         <v>10</v>
       </c>
@@ -1704,7 +1712,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19" s="12" t="s">
         <v>106</v>
       </c>
@@ -1737,7 +1745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="A20" s="11" t="s">
         <v>71</v>
       </c>
@@ -1764,7 +1772,7 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="22" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15">
       <c r="A22" s="6" t="s">
         <v>157</v>
       </c>
@@ -1775,7 +1783,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1806,7 +1814,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="28">
       <c r="A24" s="16" t="s">
         <v>102</v>
       </c>
@@ -1841,7 +1849,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="15" t="s">
         <v>158</v>
       </c>
@@ -1874,7 +1882,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="F26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1895,7 +1903,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15">
       <c r="A27" s="6" t="s">
         <v>42</v>
       </c>
@@ -1922,7 +1930,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1953,7 +1961,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="11" t="s">
         <v>20</v>
       </c>
@@ -1986,7 +1994,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2017,7 +2025,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2037,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -2041,7 +2049,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2056,7 +2064,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -2078,7 +2086,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
         <v>105</v>
       </c>
@@ -2098,7 +2106,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13">
       <c r="J36" s="1" t="s">
         <v>83</v>
       </c>
@@ -2110,7 +2118,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="15">
       <c r="A37" s="6" t="s">
         <v>55</v>
       </c>
@@ -2125,7 +2133,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>27</v>
       </c>
@@ -2147,7 +2155,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="28">
       <c r="A39" s="10" t="s">
         <v>8</v>
       </c>
@@ -2171,7 +2179,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13">
       <c r="A40" s="11" t="s">
         <v>71</v>
       </c>
@@ -2197,7 +2205,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -2221,7 +2229,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
         <v>116</v>
       </c>
@@ -2243,7 +2251,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13">
       <c r="A43" s="4" t="s">
         <v>123</v>
       </c>
@@ -2265,12 +2273,24 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13">
+      <c r="A44" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15">
       <c r="A46" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13">
       <c r="A47" s="3" t="s">
         <v>27</v>
       </c>
@@ -2282,7 +2302,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13">
       <c r="A48" s="10" t="s">
         <v>11</v>
       </c>
@@ -2296,7 +2316,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" s="11" t="s">
         <v>106</v>
       </c>
@@ -2310,7 +2330,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" s="13" t="s">
         <v>139</v>
       </c>
@@ -2324,12 +2344,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15">
       <c r="A52" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
         <v>27</v>
       </c>
@@ -2341,7 +2361,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="28">
       <c r="A54" s="16" t="s">
         <v>154</v>
       </c>
@@ -2355,7 +2375,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" s="15" t="s">
         <v>161</v>
       </c>
@@ -2367,7 +2387,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15">
       <c r="A57" s="6" t="s">
         <v>146</v>
       </c>
@@ -2375,7 +2395,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
         <v>27</v>
       </c>
@@ -2387,7 +2407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
@@ -2401,7 +2421,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" s="13" t="s">
         <v>150</v>
       </c>
@@ -2415,7 +2435,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
@@ -2427,7 +2447,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>3</v>
       </c>
@@ -2439,7 +2459,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>4</v>
       </c>
@@ -2451,7 +2471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -2463,7 +2483,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>105</v>
       </c>
@@ -2473,7 +2493,7 @@
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
-    <row r="67" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15">
       <c r="A67" s="6" t="s">
         <v>147</v>
       </c>
@@ -2481,7 +2501,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4">
       <c r="A68" s="3" t="s">
         <v>27</v>
       </c>
@@ -2493,7 +2513,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
         <v>6</v>
       </c>
@@ -2507,7 +2527,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70" s="11" t="s">
         <v>12</v>
       </c>
@@ -2521,7 +2541,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
         <v>105</v>
       </c>
@@ -2531,12 +2551,12 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="73" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15">
       <c r="A73" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
         <v>27</v>
       </c>
@@ -2548,7 +2568,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4">
       <c r="A75" s="11" t="s">
         <v>6</v>
       </c>
@@ -2562,7 +2582,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76" s="8" t="s">
         <v>117</v>
       </c>
@@ -2574,7 +2594,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4">
       <c r="A77" s="9" t="s">
         <v>118</v>
       </c>
@@ -2586,12 +2606,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="15">
       <c r="A79" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
         <v>27</v>
       </c>
@@ -2603,7 +2623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4">
       <c r="A81" s="12" t="s">
         <v>131</v>
       </c>
@@ -2617,7 +2637,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
         <v>17</v>
       </c>
@@ -2629,7 +2649,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
         <v>16</v>
       </c>
@@ -2642,7 +2662,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
1. ICommitLogCollector and GitCommitLogCollector were implemnted, tested. 2. jgit library for above implemnted modules was included.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="176">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -763,12 +763,16 @@
     <t>INT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>VARCHAR(127)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1051,20 +1055,20 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1364,10 +1368,10 @@
   <dimension ref="A1:S85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D3" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
@@ -1388,51 +1392,51 @@
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:19" ht="33.75">
+      <c r="A1" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="P1" s="17" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="P1" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-    </row>
-    <row r="2" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-    </row>
-    <row r="3" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+    </row>
+    <row r="2" spans="1:19" ht="21" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+    </row>
+    <row r="3" spans="1:19" ht="17.25">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -1446,7 +1450,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1491,7 +1495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="33">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1517,7 +1521,7 @@
         <v>106</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>126</v>
@@ -1536,7 +1540,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="33">
       <c r="A6" s="11" t="s">
         <v>111</v>
       </c>
@@ -1581,7 +1585,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="J8" s="1" t="s">
         <v>163</v>
       </c>
@@ -1646,7 +1650,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="17.25">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1674,7 +1678,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="17.25">
       <c r="A11" s="10" t="s">
         <v>100</v>
       </c>
@@ -1743,7 +1747,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="A12" s="11" t="s">
         <v>0</v>
       </c>
@@ -1786,7 +1790,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="33">
       <c r="A13" s="11" t="s">
         <v>101</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>108</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>134</v>
@@ -1831,7 +1835,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
         <v>109</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19">
       <c r="A15" s="4" t="s">
         <v>121</v>
       </c>
@@ -1893,7 +1897,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1914,7 +1918,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="17.25">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1956,7 +1960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="A20" s="10" t="s">
         <v>10</v>
       </c>
@@ -1991,7 +1995,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21" s="12" t="s">
         <v>104</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="11" t="s">
         <v>71</v>
       </c>
@@ -2051,7 +2055,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="17.25">
       <c r="A24" s="6" t="s">
         <v>155</v>
       </c>
@@ -2062,7 +2066,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -2093,7 +2097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="49.5">
       <c r="A26" s="16" t="s">
         <v>100</v>
       </c>
@@ -2128,7 +2132,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="15" t="s">
         <v>156</v>
       </c>
@@ -2161,7 +2165,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="F28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2182,7 +2186,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="17.25">
       <c r="A29" s="6" t="s">
         <v>42</v>
       </c>
@@ -2209,7 +2213,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -2240,7 +2244,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -2273,7 +2277,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="11" t="s">
         <v>13</v>
       </c>
@@ -2304,7 +2308,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -2316,7 +2320,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -2340,7 +2344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>103</v>
       </c>
@@ -2362,12 +2366,12 @@
       <c r="C37" s="4"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="17.25">
       <c r="A39" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
         <v>27</v>
       </c>
@@ -2379,7 +2383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="33">
       <c r="A41" s="10" t="s">
         <v>8</v>
       </c>
@@ -2393,7 +2397,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4">
       <c r="A42" s="11" t="s">
         <v>71</v>
       </c>
@@ -2407,7 +2411,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>114</v>
       </c>
@@ -2431,7 +2435,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
         <v>121</v>
       </c>
@@ -2443,7 +2447,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
         <v>161</v>
       </c>
@@ -2455,12 +2459,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="17.25">
       <c r="A48" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
         <v>27</v>
       </c>
@@ -2472,7 +2476,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" s="10" t="s">
         <v>11</v>
       </c>
@@ -2486,7 +2490,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" s="11" t="s">
         <v>104</v>
       </c>
@@ -2500,7 +2504,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" s="13" t="s">
         <v>137</v>
       </c>
@@ -2514,12 +2518,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="17.25">
       <c r="A54" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
         <v>27</v>
       </c>
@@ -2531,7 +2535,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="33">
       <c r="A56" s="16" t="s">
         <v>152</v>
       </c>
@@ -2545,7 +2549,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57" s="15" t="s">
         <v>159</v>
       </c>
@@ -2557,7 +2561,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="17.25">
       <c r="A59" s="6" t="s">
         <v>144</v>
       </c>
@@ -2565,7 +2569,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
         <v>27</v>
       </c>
@@ -2577,7 +2581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61" s="11" t="s">
         <v>6</v>
       </c>
@@ -2591,7 +2595,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4">
       <c r="A62" s="13" t="s">
         <v>148</v>
       </c>
@@ -2605,7 +2609,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -2617,7 +2621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
@@ -2629,7 +2633,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
@@ -2641,7 +2645,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -2653,7 +2657,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
         <v>103</v>
       </c>
@@ -2663,7 +2667,7 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="69" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="17.25">
       <c r="A69" s="6" t="s">
         <v>145</v>
       </c>
@@ -2671,7 +2675,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
         <v>27</v>
       </c>
@@ -2683,7 +2687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" s="11" t="s">
         <v>6</v>
       </c>
@@ -2697,7 +2701,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4">
       <c r="A72" s="11" t="s">
         <v>12</v>
       </c>
@@ -2711,7 +2715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
         <v>103</v>
       </c>
@@ -2721,12 +2725,12 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="75" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="17.25">
       <c r="A75" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
         <v>27</v>
       </c>
@@ -2738,7 +2742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4">
       <c r="A77" s="11" t="s">
         <v>6</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4">
       <c r="A78" s="8" t="s">
         <v>115</v>
       </c>
@@ -2764,7 +2768,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4">
       <c r="A79" s="9" t="s">
         <v>116</v>
       </c>
@@ -2776,12 +2780,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="17.25">
       <c r="A81" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
         <v>27</v>
       </c>
@@ -2793,7 +2797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4">
       <c r="A83" s="12" t="s">
         <v>129</v>
       </c>
@@ -2807,7 +2811,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
         <v>17</v>
       </c>
@@ -2819,7 +2823,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
GitCommitLogCollector, ScmRepoAnalyzer implemented and tested.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="180">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -767,12 +767,28 @@
     <t>VARCHAR(127)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Commit log's score</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_SCORE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPEN_DATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug submitted date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1365,13 +1381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S85"/>
+  <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
@@ -1392,7 +1408,7 @@
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="33.75">
+    <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>169</v>
       </c>
@@ -1415,7 +1431,7 @@
       <c r="R1" s="21"/>
       <c r="S1" s="21"/>
     </row>
-    <row r="2" spans="1:19" ht="21" customHeight="1">
+    <row r="2" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1436,7 +1452,7 @@
       <c r="R2" s="18"/>
       <c r="S2" s="18"/>
     </row>
-    <row r="3" spans="1:19" ht="17.25">
+    <row r="3" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -1450,7 +1466,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1495,7 +1511,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="33">
+    <row r="5" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1540,7 +1556,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="33">
+    <row r="6" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>111</v>
       </c>
@@ -1585,7 +1601,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -1628,7 +1644,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J8" s="1" t="s">
         <v>163</v>
       </c>
@@ -1650,7 +1666,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="17.25">
+    <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1678,7 +1694,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1711,7 +1727,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="17.25">
+    <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>100</v>
       </c>
@@ -1747,7 +1763,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>0</v>
       </c>
@@ -1790,7 +1806,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="33">
+    <row r="13" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>101</v>
       </c>
@@ -1835,7 +1851,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>109</v>
       </c>
@@ -1866,7 +1882,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>121</v>
       </c>
@@ -1897,7 +1913,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1918,7 +1934,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="17.25">
+    <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -1929,7 +1945,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1960,7 +1976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>10</v>
       </c>
@@ -1995,7 +2011,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>104</v>
       </c>
@@ -2028,7 +2044,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>71</v>
       </c>
@@ -2055,7 +2071,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="24" spans="1:13" ht="17.25">
+    <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>155</v>
       </c>
@@ -2066,7 +2082,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -2097,7 +2113,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="49.5">
+    <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>100</v>
       </c>
@@ -2132,7 +2148,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>156</v>
       </c>
@@ -2165,7 +2181,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2186,7 +2202,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="17.25">
+    <row r="29" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>42</v>
       </c>
@@ -2213,7 +2229,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -2244,7 +2260,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -2277,7 +2293,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>13</v>
       </c>
@@ -2298,17 +2314,17 @@
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>112</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -2319,8 +2335,18 @@
       <c r="D33" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="J33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="M33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -2332,7 +2358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -2344,7 +2370,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -2356,7 +2382,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>103</v>
       </c>
@@ -2366,12 +2392,12 @@
       <c r="C37" s="4"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="17.25">
+    <row r="39" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>27</v>
       </c>
@@ -2383,7 +2409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="33">
+    <row r="41" spans="1:13" ht="33" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>8</v>
       </c>
@@ -2397,7 +2423,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>71</v>
       </c>
@@ -2411,427 +2437,439 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>7</v>
+        <v>178</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="4" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1" t="s">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25">
-      <c r="A48" s="6" t="s">
+    <row r="49" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="3" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="10" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="11" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="13" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25">
-      <c r="A54" s="6" t="s">
+    <row r="55" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3" t="s">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="33">
-      <c r="A56" s="16" t="s">
+    <row r="57" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A57" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="15" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4" t="s">
+      <c r="C58" s="4"/>
+      <c r="D58" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25">
-      <c r="A59" s="6" t="s">
+    <row r="60" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="3" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3" t="s">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="11" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1" t="s">
-        <v>2</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="D63" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" s="4"/>
+      <c r="D67" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-    </row>
-    <row r="69" spans="1:4" ht="17.25">
-      <c r="A69" s="6" t="s">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+    </row>
+    <row r="70" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="3" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3" t="s">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="11" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-    </row>
-    <row r="75" spans="1:4" ht="17.25">
-      <c r="A75" s="6" t="s">
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+    </row>
+    <row r="76" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="3" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="11" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25">
-      <c r="A81" s="6" t="s">
+    <row r="82" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="3" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="12" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C84" s="1"/>
+      <c r="C84" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="D84" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
[In progress] implement extraction of structured information from source files
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="193">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -195,10 +195,6 @@
   </si>
   <si>
     <t>Corpus from source file</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_ANALYSIS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -596,10 +592,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>UNIQUE COMP_IDX_SF_ANALYSIS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>UNIQUE IDX_SF_COR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -613,14 +605,6 @@
   </si>
   <si>
     <t>IDX_BUG_COR_PROD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_SF_ANALYSIS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_ANALYSIS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -660,10 +644,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Bug와 Source File의 corpus 간의 분석</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>IDX_INT_ANAL_BUG_ID,
 UNIQUE COMP_IDX_INT_ANALSYS</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -781,6 +761,78 @@
   </si>
   <si>
     <t>Bug submitted date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug와 Source File의 corpus 간의 분석, Bug report의 corpus에 대한 Source file의 vector값을 찾아냄.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_SF_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAR_COR_SET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_COR_SET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLS_COR_SET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMT_COR_SET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class corpus set</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method corpus set</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable corpus set</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment corpus set</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DESC_COR_SET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMR_COR_SET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summary corpus set</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description corpus set</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_SF_VEC</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1381,17 +1433,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S86"/>
+  <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.125" customWidth="1"/>
     <col min="5" max="5" width="6.125" customWidth="1"/>
     <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
@@ -1410,7 +1462,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -1425,7 +1477,7 @@
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="P1" s="20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
@@ -1457,13 +1509,13 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1474,7 +1526,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>29</v>
@@ -1495,7 +1547,7 @@
         <v>28</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>29</v>
@@ -1516,10 +1568,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
@@ -1528,43 +1580,43 @@
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
@@ -1573,97 +1625,97 @@
         <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J8" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
@@ -1671,27 +1723,27 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1715,52 +1767,52 @@
         <v>29</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1768,10 +1820,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>31</v>
@@ -1780,10 +1832,10 @@
         <v>19</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>27</v>
@@ -1796,165 +1848,184 @@
         <v>29</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="J15" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="7"/>
+        <v>181</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>185</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
     <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>39</v>
+      <c r="A18" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
-        <v>29</v>
+      <c r="A19" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>27</v>
@@ -1977,121 +2048,121 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>155</v>
+      <c r="A24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>29</v>
+      <c r="A25" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>27</v>
@@ -2114,451 +2185,449 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>100</v>
+      <c r="A26" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="F27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J27" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" t="s">
-        <v>147</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
-        <v>29</v>
+      <c r="A30" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>20</v>
+      <c r="A31" s="15" t="s">
+        <v>151</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>43</v>
+      <c r="B33" t="s">
+        <v>143</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>44</v>
+      <c r="A34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="4"/>
+      <c r="A35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="4"/>
+      <c r="A36" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="D36" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="43" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="39" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="33" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>58</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
-        <v>29</v>
+      <c r="A50" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
-        <v>11</v>
+      <c r="A51" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>126</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>59</v>
+      <c r="A52" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>137</v>
+      <c r="A53" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>153</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2573,199 +2642,203 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
-        <v>152</v>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>72</v>
+        <v>125</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B58" s="4" t="s">
+      <c r="A58" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
+      <c r="C59" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A63" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B66" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B60" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="B69" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1" t="s">
+      <c r="B70" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="1" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-    </row>
-    <row r="70" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B70" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
     <row r="76" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>62</v>
+        <v>177</v>
+      </c>
+      <c r="B76" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2785,42 +2858,42 @@
         <v>6</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="8" t="s">
-        <v>115</v>
+      <c r="A79" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C79" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D79" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="9" t="s">
-        <v>116</v>
+      <c r="A80" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C80" s="1"/>
-      <c r="D80" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="D80" s="1"/>
     </row>
     <row r="82" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2836,40 +2909,95 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="12" t="s">
-        <v>129</v>
+      <c r="A84" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>17</v>
+      <c r="A85" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+      <c r="B92" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
SIMI_SCORE, STRACE_SCORE, COMM_SCORE verified.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="199">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -66,22 +66,6 @@
   </si>
   <si>
     <t>SF_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_COR_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_COR_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_COR_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_COR_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -186,15 +170,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SF_COR_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Corpus ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Corpus from source file</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -259,18 +235,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>BUG_COR_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Corpus from bug report</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SIMI_BUG_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Similar bug ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -465,8 +429,275 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>COR_SET</t>
+  </si>
+  <si>
+    <t>SF_NAME(Unique)</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>FIXED_SF_VER_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIXED_FUNC_VER_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_DATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_VER_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source file &amp; version ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>TOT_CNT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total corpus count</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP_IDX_SF_VER_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_FIX_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_SIMI_BUG_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDX_SF_INFO_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_SF_PROD_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_COMM_PROD_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_COMM_FILE_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_EXP_INFO_PROD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_EXP_INFO_ALG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROD_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_ANALYSIS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug와 Bug 간의 분석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source File과 Souce File의 corpus 간의 분석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_INT_ANAL_BUG_ID,
+UNIQUE COMP_IDX_INT_ANALSYS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_INT_ANALSYS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_ID(KEY)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_STRACE_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imported class in the source file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_IMP_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMP_CLASS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_SF_IMP_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_STRACE_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>STRACE_CLASS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class in stack-trace from bug report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VER</t>
+  </si>
+  <si>
+    <t>COMM_TYPE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commit message</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commit type(Add, Change, Delete)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(63)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMITTER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commmitter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tables for Bug Localization</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tables for Evalution of BL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_FILE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commited file name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(127)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commit log's score</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_SCORE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPEN_DATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug submitted date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug와 Source File의 corpus 간의 분석, Bug report의 corpus에 대한 Source file의 vector값을 찾아냄.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_SF_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_SF_VEC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WRD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word from source file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t>COR</t>
+      <t>W</t>
     </r>
     <r>
       <rPr>
@@ -477,147 +708,29 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>_SET</t>
+      <t>RD</t>
     </r>
-  </si>
-  <si>
-    <t>COR_SET</t>
-  </si>
-  <si>
-    <t>SF_NAME(Unique)</t>
-  </si>
-  <si>
-    <t>DOUBLE</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIXED_SF_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIXED_FUNC_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMM_DATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source file &amp; version ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR</t>
-  </si>
-  <si>
-    <t>TOT_CNT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total corpus count</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Index</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMP_IDX_SF_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRIMARY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_BUG_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_BUG_FIX_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_SIMI_BUG_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE IDX_SF_INFO_NAME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_SF_PROD_NAME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_COMM_PROD_NAME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_COMM_FILE_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_EXP_INFO_PROD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_EXP_INFO_ALG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PROD_NAME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE COMP_IDX_BUG_ANALYSIS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE IDX_SF_COR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_SF_COR_PROD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE IDC_BUG_COR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_BUG_COR_PROD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug와 Bug 간의 분석</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source File과 Souce File의 corpus 간의 분석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word from bug report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDX_SF_WRD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_WRD_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_WRD_ID(KEY)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>S</t>
+      <t>SF_</t>
     </r>
     <r>
       <rPr>
@@ -628,7 +741,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>F</t>
+      <t>WRD</t>
     </r>
     <r>
       <rPr>
@@ -639,200 +752,136 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>_COR_ID</t>
+      <t>_ID</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>IDX_INT_ANAL_BUG_ID,
-UNIQUE COMP_IDX_INT_ANALSYS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE COMP_IDX_INT_ANALSYS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_STRACE_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Imported class in the source file</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_IMP_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IMP_CLASS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_SF_IMP_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_BUG_STRACE_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>STRACE_CLASS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Class in stack-trace from bug report</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VER</t>
-  </si>
-  <si>
-    <t>COMM_TYPE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commit message</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commit type(Add, Change, Delete)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(63)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMMITTER</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commmitter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tables for Bug Localization</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tables for Evalution of BL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMM_FILE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(255)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commited file name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(127)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commit log's score</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMM_SCORE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OPEN_DATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug submitted date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug와 Source File의 corpus 간의 분석, Bug report의 corpus에 대한 Source file의 vector값을 찾아냄.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE COMP_IDX_SF_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE COMP_IDX_BUG_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VAR_COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MTH_COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CLS_COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMT_COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Class corpus set</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Method corpus set</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Variable corpus set</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comment corpus set</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DESC_COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMR_COR_SET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Summary corpus set</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description corpus set</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_SF_VEC</t>
+    <t>BUG_WRD_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_WRD_ID(KEY)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug word ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source file word ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDC_BUG_WRD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_WRD_PROD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_WRD_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>BUG_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WRD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_ID</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLS_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAR_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMT_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_SF_WRD_PROD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMR_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DESC_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summary corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total word count</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIMI_BUG_ANALYSIS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1071,7 +1120,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1130,6 +1179,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="12" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
@@ -1435,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1461,27 +1513,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="P1" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="A1" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="P1" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
@@ -1506,61 +1558,61 @@
     </row>
     <row r="3" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="33" x14ac:dyDescent="0.3">
@@ -1568,251 +1620,251 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="Q7" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J8" s="1" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="4" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="P11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1820,118 +1872,118 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>107</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>186</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -1939,112 +1991,112 @@
         <v>182</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="4" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>122</v>
+        <v>197</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2052,67 +2104,67 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F21" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>39</v>
+        <v>170</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -2121,321 +2173,321 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>103</v>
+      <c r="A25" s="20" t="s">
+        <v>165</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>166</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F32" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
-        <v>13</v>
+      <c r="A36" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -2443,11 +2495,11 @@
         <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2455,11 +2507,11 @@
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2467,11 +2519,11 @@
         <v>4</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -2479,38 +2531,38 @@
         <v>5</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="1"/>
     </row>
     <row r="43" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="33" x14ac:dyDescent="0.3">
@@ -2518,39 +2570,39 @@
         <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -2558,193 +2610,193 @@
         <v>7</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>113</v>
+        <v>192</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>37</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>122</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>57</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="11" t="s">
-        <v>103</v>
+      <c r="A58" s="13" t="s">
+        <v>167</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="15" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B66" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2752,27 +2804,27 @@
         <v>6</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -2780,11 +2832,11 @@
         <v>2</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -2792,11 +2844,11 @@
         <v>3</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2804,11 +2856,11 @@
         <v>4</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2816,41 +2868,41 @@
         <v>5</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
     <row r="76" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2858,54 +2910,54 @@
         <v>6</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="11" t="s">
-        <v>12</v>
+      <c r="A79" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
     <row r="82" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2913,88 +2965,88 @@
         <v>6</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>

</xml_diff>

<commit_message>
1. VSM_SCORE logic verified. 2. NORM columns for source file and bug table added. 3. Vector name changed to Term Weight.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="213">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -532,10 +532,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>UNIQUE COMP_IDX_BUG_ANALYSIS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Bug와 Bug 간의 분석</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -668,111 +664,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SF_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE COMP_IDX_SF_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE COMP_IDX_BUG_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_SF_VEC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WRD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word from source file</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RD</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word from bug report</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE IDX_SF_WRD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_WRD_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SF_WRD_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>SF_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WRD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_ID</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_WRD_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUG_WRD_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug word ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source file word ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>UNIQUE IDC_BUG_WRD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -781,38 +672,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SF_WRD_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>BUG_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WRD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_ID</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>COR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -853,10 +712,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>IDX_SF_WRD_PROD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>COR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -877,11 +732,151 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Total word count</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SIMI_BUG_ANALYSIS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_TERM_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_TERM_ID(KEY)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source file term ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_TERM_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_TERM_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_TERM_ID(KEY)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug term ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term from bug report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TERM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_TERM_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDX_SF_TERM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_SF_TERM_PROD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term weight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COR_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLS_COR_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_COR_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMT_COR_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAR_COR_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of class corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of method corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of variable corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of comment corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMR_COR_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DESC_COR_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of summary corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of description corpus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total term count</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term from source file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_SF_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_SF_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_SF_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_TERM_WGT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1120,7 +1115,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1189,6 +1184,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1485,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S92"/>
+  <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1514,7 +1512,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1529,7 +1527,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
       <c r="P1" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q1" s="22"/>
       <c r="R1" s="22"/>
@@ -1641,7 +1639,7 @@
         <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>114</v>
@@ -1750,14 +1748,14 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>108</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>69</v>
@@ -1778,14 +1776,14 @@
         <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>70</v>
@@ -1936,7 +1934,7 @@
         <v>98</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>122</v>
@@ -1957,14 +1955,14 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>99</v>
@@ -1976,26 +1974,26 @@
         <v>33</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>109</v>
@@ -2007,26 +2005,26 @@
         <v>111</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
@@ -2040,26 +2038,26 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
@@ -2077,7 +2075,7 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>23</v>
@@ -2133,6 +2131,16 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>94</v>
       </c>
@@ -2153,9 +2161,16 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>170</v>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>61</v>
@@ -2172,29 +2187,27 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>25</v>
+      <c r="A23" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>176</v>
+      <c r="A24" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="F24" t="s">
         <v>47</v>
@@ -2204,17 +2217,15 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>166</v>
+      <c r="A25" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>23</v>
@@ -2237,18 +2248,6 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F26" s="1" t="s">
         <v>19</v>
       </c>
@@ -2265,13 +2264,16 @@
         <v>88</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>177</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>21</v>
       </c>
@@ -2288,15 +2290,22 @@
         <v>86</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>134</v>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
@@ -2319,15 +2328,17 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
-        <v>25</v>
+      <c r="A29" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3</v>
@@ -2350,17 +2361,17 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>90</v>
+      <c r="A30" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>27</v>
+        <v>206</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>4</v>
@@ -2383,15 +2394,17 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>135</v>
+      <c r="A31" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="D31" s="1" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>5</v>
@@ -2422,22 +2435,19 @@
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>101</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B33" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>22</v>
@@ -2463,489 +2473,496 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>16</v>
+      <c r="A35" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>162</v>
+      <c r="C35" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="B36" s="1" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="C41" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1" t="s">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="1" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="1" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="43" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
+    <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="33" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
+    <row r="49" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4" t="s">
-        <v>197</v>
+      <c r="A52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>140</v>
+      <c r="A53" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
+    <row r="62" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3" t="s">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="B57" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="D64" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
+      <c r="C65" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D59" s="1" t="s">
+      <c r="C66" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
+    <row r="68" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A63" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B63" s="1" t="s">
+    <row r="70" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A70" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="15" t="s">
+      <c r="B71" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B66" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
+    </row>
+    <row r="73" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A73" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3" t="s">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D68" s="1" t="s">
+      <c r="C75" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="13" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B69" s="1" t="s">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1" t="s">
+      <c r="C78" s="1"/>
+      <c r="D78" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="1" t="s">
+      <c r="C79" s="4"/>
+      <c r="D79" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-    </row>
-    <row r="76" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B76" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="82" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>52</v>
+        <v>212</v>
+      </c>
+      <c r="B82" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2968,39 +2985,41 @@
         <v>88</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>116</v>
+        <v>210</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="8" t="s">
-        <v>103</v>
+      <c r="A85" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="1"/>
+      <c r="C85" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="D85" s="1" t="s">
-        <v>27</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1" t="s">
-        <v>40</v>
+      <c r="A86" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>198</v>
+        <v>52</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -3016,40 +3035,95 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="12" t="s">
-        <v>117</v>
+      <c r="A90" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>13</v>
+      <c r="A91" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Database creation policy changed.(One DB for all projects to one DB for one project)
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="135" yWindow="75" windowWidth="27945" windowHeight="17460"/>
+    <workbookView xWindow="135" yWindow="75" windowWidth="27945" windowHeight="17460" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DB schema design" sheetId="1" r:id="rId1"/>
+    <sheet name="Analysis DB" sheetId="1" r:id="rId1"/>
+    <sheet name="Evaluation DB" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="223">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -616,10 +617,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Tables for Bug Localization</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Tables for Evalution of BL</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -877,6 +874,50 @@
   </si>
   <si>
     <t>BUG_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALPHA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BETA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAST_DAYS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP1_RATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP5_RATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP10_RATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top 1 ranked rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top 5 ranked rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top 10 ranked rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tables for BLIA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1179,14 +1220,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="12" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1483,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S98"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1504,36 +1545,26 @@
     <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="P1" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-    </row>
-    <row r="2" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+    </row>
+    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1548,13 +1579,8 @@
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
       <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-    </row>
-    <row r="3" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -1564,11 +1590,8 @@
       <c r="J3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1602,18 +1625,8 @@
       <c r="M4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1639,7 +1652,7 @@
         <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>114</v>
@@ -1647,18 +1660,8 @@
       <c r="M5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>100</v>
       </c>
@@ -1692,18 +1695,8 @@
       <c r="M6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>61</v>
       </c>
@@ -1735,18 +1728,8 @@
       <c r="M7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J8" s="1" t="s">
         <v>141</v>
       </c>
@@ -1757,18 +1740,8 @@
       <c r="M8" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="R8" s="4"/>
-      <c r="S8" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1785,18 +1758,8 @@
       <c r="M9" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="R9" s="4"/>
-      <c r="S9" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1816,20 +1779,8 @@
       <c r="H10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>90</v>
       </c>
@@ -1852,20 +1803,8 @@
       <c r="J11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>0</v>
       </c>
@@ -1897,18 +1836,8 @@
       <c r="M12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>91</v>
       </c>
@@ -1934,7 +1863,7 @@
         <v>98</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>122</v>
@@ -1942,27 +1871,17 @@
       <c r="M13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="P13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>99</v>
@@ -1974,26 +1893,26 @@
         <v>33</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>109</v>
@@ -2008,23 +1927,23 @@
         <v>140</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
@@ -2038,26 +1957,26 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
@@ -2075,7 +1994,7 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>23</v>
@@ -2132,14 +2051,14 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>94</v>
@@ -2163,14 +2082,14 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B22" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>61</v>
@@ -2188,26 +2107,26 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B23" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="B24" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F24" t="s">
         <v>47</v>
@@ -2218,14 +2137,14 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>23</v>
@@ -2272,7 +2191,7 @@
     </row>
     <row r="27" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>21</v>
@@ -2329,7 +2248,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>86</v>
@@ -2338,7 +2257,7 @@
         <v>114</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3</v>
@@ -2362,16 +2281,16 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>4</v>
@@ -2401,7 +2320,7 @@
         <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>60</v>
@@ -2435,14 +2354,14 @@
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>101</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
@@ -2500,7 +2419,7 @@
     </row>
     <row r="38" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B38" t="s">
         <v>127</v>
@@ -2526,7 +2445,7 @@
         <v>86</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>31</v>
@@ -2534,16 +2453,16 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -2641,14 +2560,14 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2665,38 +2584,38 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2708,43 +2627,43 @@
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B57" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B58" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B59" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="B59" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2761,7 +2680,7 @@
     </row>
     <row r="62" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2778,7 +2697,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>86</v>
@@ -2787,21 +2706,21 @@
         <v>114</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2812,7 +2731,7 @@
         <v>88</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>60</v>
@@ -2863,10 +2782,10 @@
     </row>
     <row r="73" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B73" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2889,7 +2808,7 @@
         <v>88</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>49</v>
@@ -2897,16 +2816,16 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2959,7 +2878,7 @@
     </row>
     <row r="82" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B82" t="s">
         <v>126</v>
@@ -2985,7 +2904,7 @@
         <v>88</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>49</v>
@@ -2993,28 +2912,28 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
@@ -3074,7 +2993,7 @@
     </row>
     <row r="94" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -3126,9 +3045,8 @@
       <c r="D98" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
-    <mergeCell ref="P1:S1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3139,4 +3057,238 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Evaluation property modified. Debug codes added.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaus\Dropbox\Workspace\BLIA\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="135" yWindow="75" windowWidth="27945" windowHeight="17460" activeTab="1"/>
+    <workbookView minimized="1" xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis DB" sheetId="1" r:id="rId1"/>
@@ -17,11 +12,11 @@
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -929,7 +924,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -937,14 +932,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -953,7 +948,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -962,7 +957,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -970,7 +965,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -984,7 +979,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -992,7 +987,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1000,14 +995,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1015,7 +1010,7 @@
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1023,7 +1018,7 @@
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1231,22 +1226,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="40% - 강조색2" xfId="12" builtinId="35"/>
-    <cellStyle name="강조색2" xfId="11" builtinId="33"/>
-    <cellStyle name="메모" xfId="15" builtinId="10"/>
-    <cellStyle name="보통" xfId="1" builtinId="28"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="좋음" xfId="6" builtinId="26"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="40% - Accent2" xfId="12" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="11" builtinId="33"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1516,7 +1511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1526,28 +1521,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.125" customWidth="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1"/>
-    <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" customWidth="1"/>
-    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="28">
       <c r="A1" s="22" t="s">
         <v>221</v>
       </c>
@@ -1564,7 +1558,7 @@
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
     </row>
-    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="21" customHeight="1">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1580,7 +1574,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -1591,7 +1585,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1626,7 +1620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="28">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1661,7 +1655,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="28">
       <c r="A6" s="11" t="s">
         <v>100</v>
       </c>
@@ -1696,7 +1690,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
         <v>61</v>
       </c>
@@ -1729,7 +1723,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14">
       <c r="J8" s="1" t="s">
         <v>141</v>
       </c>
@@ -1741,7 +1735,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1759,7 +1753,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1780,7 +1774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15">
       <c r="A11" s="10" t="s">
         <v>90</v>
       </c>
@@ -1804,7 +1798,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14">
       <c r="A12" s="11" t="s">
         <v>0</v>
       </c>
@@ -1837,7 +1831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="28">
       <c r="A13" s="11" t="s">
         <v>91</v>
       </c>
@@ -1872,7 +1866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>160</v>
       </c>
@@ -1903,7 +1897,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>161</v>
       </c>
@@ -1934,7 +1928,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>162</v>
       </c>
@@ -1955,7 +1949,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>163</v>
       </c>
@@ -1967,7 +1961,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15">
       <c r="A18" s="1" t="s">
         <v>164</v>
       </c>
@@ -1985,7 +1979,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
         <v>109</v>
       </c>
@@ -2016,7 +2010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -2049,7 +2043,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
         <v>190</v>
       </c>
@@ -2080,7 +2074,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
         <v>191</v>
       </c>
@@ -2105,7 +2099,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
         <v>192</v>
       </c>
@@ -2117,7 +2111,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15">
       <c r="A24" s="4" t="s">
         <v>194</v>
       </c>
@@ -2135,7 +2129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="4" t="s">
         <v>193</v>
       </c>
@@ -2166,7 +2160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="28">
       <c r="F26" s="1" t="s">
         <v>19</v>
       </c>
@@ -2189,7 +2183,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15">
       <c r="A27" s="6" t="s">
         <v>176</v>
       </c>
@@ -2215,7 +2209,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
@@ -2246,7 +2240,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="10" t="s">
         <v>177</v>
       </c>
@@ -2279,7 +2273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="20" t="s">
         <v>184</v>
       </c>
@@ -2312,7 +2306,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="11" t="s">
         <v>61</v>
       </c>
@@ -2345,7 +2339,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="F32" s="1" t="s">
         <v>93</v>
       </c>
@@ -2364,7 +2358,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15">
       <c r="A33" s="6" t="s">
         <v>133</v>
       </c>
@@ -2379,7 +2373,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>23</v>
       </c>
@@ -2391,7 +2385,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13">
       <c r="A35" s="16" t="s">
         <v>90</v>
       </c>
@@ -2405,7 +2399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13">
       <c r="A36" s="15" t="s">
         <v>134</v>
       </c>
@@ -2417,7 +2411,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="15">
       <c r="A38" s="6" t="s">
         <v>206</v>
       </c>
@@ -2425,7 +2419,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>23</v>
       </c>
@@ -2437,7 +2431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13">
       <c r="A40" s="11" t="s">
         <v>16</v>
       </c>
@@ -2451,7 +2445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13">
       <c r="A41" s="13" t="s">
         <v>179</v>
       </c>
@@ -2465,7 +2459,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
@@ -2477,7 +2471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -2489,7 +2483,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
@@ -2501,7 +2495,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -2513,12 +2507,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="15">
       <c r="A47" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13">
       <c r="A48" s="3" t="s">
         <v>23</v>
       </c>
@@ -2530,7 +2524,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="28">
       <c r="A49" s="10" t="s">
         <v>8</v>
       </c>
@@ -2544,7 +2538,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" s="11" t="s">
         <v>61</v>
       </c>
@@ -2558,7 +2552,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>155</v>
       </c>
@@ -2570,7 +2564,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2582,7 +2576,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>170</v>
       </c>
@@ -2594,7 +2588,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>171</v>
       </c>
@@ -2606,7 +2600,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>172</v>
       </c>
@@ -2618,7 +2612,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
         <v>109</v>
       </c>
@@ -2630,7 +2624,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57" s="4" t="s">
         <v>190</v>
       </c>
@@ -2642,7 +2636,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58" s="4" t="s">
         <v>200</v>
       </c>
@@ -2654,7 +2648,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59" s="4" t="s">
         <v>201</v>
       </c>
@@ -2666,7 +2660,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" s="4" t="s">
         <v>139</v>
       </c>
@@ -2678,12 +2672,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15">
       <c r="A62" s="6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63" s="3" t="s">
         <v>23</v>
       </c>
@@ -2695,7 +2689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" s="10" t="s">
         <v>181</v>
       </c>
@@ -2709,7 +2703,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" s="13" t="s">
         <v>184</v>
       </c>
@@ -2723,7 +2717,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66" s="13" t="s">
         <v>125</v>
       </c>
@@ -2737,12 +2731,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15">
       <c r="A68" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4">
       <c r="A69" s="3" t="s">
         <v>23</v>
       </c>
@@ -2754,7 +2748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="28">
       <c r="A70" s="16" t="s">
         <v>130</v>
       </c>
@@ -2768,7 +2762,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" s="15" t="s">
         <v>137</v>
       </c>
@@ -2780,7 +2774,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15">
       <c r="A73" s="6" t="s">
         <v>208</v>
       </c>
@@ -2788,7 +2782,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
         <v>23</v>
       </c>
@@ -2800,7 +2794,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4">
       <c r="A75" s="11" t="s">
         <v>6</v>
       </c>
@@ -2814,7 +2808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76" s="13" t="s">
         <v>179</v>
       </c>
@@ -2828,7 +2822,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
@@ -2840,7 +2834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
         <v>3</v>
       </c>
@@ -2852,7 +2846,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
         <v>4</v>
       </c>
@@ -2864,7 +2858,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
@@ -2876,7 +2870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="15">
       <c r="A82" s="6" t="s">
         <v>211</v>
       </c>
@@ -2884,7 +2878,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4">
       <c r="A83" s="3" t="s">
         <v>23</v>
       </c>
@@ -2896,7 +2890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4">
       <c r="A84" s="11" t="s">
         <v>6</v>
       </c>
@@ -2910,7 +2904,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4">
       <c r="A85" s="13" t="s">
         <v>185</v>
       </c>
@@ -2924,7 +2918,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
         <v>188</v>
       </c>
@@ -2936,12 +2930,12 @@
         <v>189</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="15">
       <c r="A88" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
         <v>23</v>
       </c>
@@ -2953,7 +2947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4">
       <c r="A90" s="11" t="s">
         <v>6</v>
       </c>
@@ -2967,7 +2961,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4">
       <c r="A91" s="8" t="s">
         <v>103</v>
       </c>
@@ -2979,7 +2973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4">
       <c r="A92" s="9" t="s">
         <v>104</v>
       </c>
@@ -2991,12 +2985,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="15">
       <c r="A94" s="6" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4">
       <c r="A95" s="3" t="s">
         <v>23</v>
       </c>
@@ -3008,7 +3002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4">
       <c r="A96" s="12" t="s">
         <v>117</v>
       </c>
@@ -3022,7 +3016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
         <v>13</v>
       </c>
@@ -3034,7 +3028,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4">
       <c r="A98" s="1" t="s">
         <v>12</v>
       </c>
@@ -3050,7 +3044,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3063,19 +3057,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28">
       <c r="A1" s="22" t="s">
         <v>147</v>
       </c>
@@ -3083,18 +3077,18 @@
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -3106,7 +3100,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -3118,7 +3112,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3130,7 +3124,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -3142,7 +3136,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>215</v>
       </c>
@@ -3154,7 +3148,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>216</v>
       </c>
@@ -3166,7 +3160,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>217</v>
       </c>
@@ -3178,7 +3172,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -3190,7 +3184,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -3202,7 +3196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="11" t="s">
         <v>61</v>
       </c>
@@ -3216,7 +3210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="11" t="s">
         <v>74</v>
       </c>
@@ -3230,7 +3224,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
         <v>75</v>
       </c>
@@ -3242,7 +3236,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
         <v>212</v>
       </c>
@@ -3252,7 +3246,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
         <v>213</v>
       </c>
@@ -3262,7 +3256,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
         <v>214</v>
       </c>
@@ -3272,7 +3266,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
         <v>76</v>
       </c>
@@ -3290,5 +3284,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. File path handling logic added to include test sources 2. Improved stack trace analysis logic to support file path 3. Same fixed date handling logic added for computing similarity score among bug reports 4. DB schema updated(SF_INFO.CLS_NAME added. BUG_INFO.IDX_BUG_INFO_FDATE)
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaus\Dropbox\Workspace\BLIA\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="14505"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis DB" sheetId="1" r:id="rId1"/>
@@ -12,18 +17,18 @@
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="227">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -484,10 +489,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>IDX_BUG_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>IDX_BUG_FIX_INFO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -497,10 +498,6 @@
   </si>
   <si>
     <t>IDX_SIMI_BUG_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE IDX_SF_INFO_NAME</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -913,6 +910,30 @@
   </si>
   <si>
     <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDX_SF_INFO_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLS_NAME(Unique)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDX_SF_INFO_CLS_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_INFO_PROD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_INFO_FDATE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -924,7 +945,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -932,14 +953,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -948,7 +969,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -957,7 +978,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -965,7 +986,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -979,7 +1000,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -987,7 +1008,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -995,14 +1016,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1010,7 +1031,7 @@
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1018,7 +1039,7 @@
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1226,22 +1247,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="40% - Accent2" xfId="12" builtinId="35"/>
-    <cellStyle name="Accent2" xfId="11" builtinId="33"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10"/>
+    <cellStyle name="40% - 강조색2" xfId="12" builtinId="35"/>
+    <cellStyle name="강조색2" xfId="11" builtinId="33"/>
+    <cellStyle name="메모" xfId="15" builtinId="10"/>
+    <cellStyle name="보통" xfId="1" builtinId="28"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="좋음" xfId="6" builtinId="26"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="13" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1511,7 +1532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1519,31 +1540,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N98"/>
+  <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.125" customWidth="1"/>
+    <col min="5" max="5" width="6.125" customWidth="1"/>
+    <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.625" customWidth="1"/>
+    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28">
+    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1558,7 +1579,7 @@
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
     </row>
-    <row r="2" spans="1:14" ht="21" customHeight="1">
+    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1574,7 +1595,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:14" ht="15">
+    <row r="3" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -1585,7 +1606,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1620,7 +1641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28">
+    <row r="5" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1646,7 +1667,7 @@
         <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>114</v>
@@ -1655,7 +1676,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="28">
+    <row r="6" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>100</v>
       </c>
@@ -1663,7 +1684,7 @@
         <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>221</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>29</v>
@@ -1684,24 +1705,24 @@
         <v>28</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="11" t="s">
-        <v>61</v>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>222</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>120</v>
+        <v>223</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>61</v>
@@ -1723,46 +1744,48 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>108</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15">
-      <c r="A9" s="6" t="s">
-        <v>30</v>
-      </c>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>23</v>
@@ -1774,17 +1797,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15">
-      <c r="A11" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="1"/>
+    <row r="11" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1798,19 +1821,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="11" t="s">
-        <v>0</v>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1831,18 +1852,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="28">
+    <row r="13" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>91</v>
@@ -1857,25 +1878,27 @@
         <v>98</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="1" t="s">
-        <v>160</v>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>99</v>
@@ -1887,26 +1910,26 @@
         <v>33</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>109</v>
@@ -1918,26 +1941,26 @@
         <v>111</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
@@ -1949,28 +1972,28 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
@@ -1979,16 +2002,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
-        <v>204</v>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>23</v>
@@ -2010,16 +2033,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="1" t="s">
-        <v>34</v>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
@@ -2043,16 +2066,16 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" s="21" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>195</v>
+      <c r="C21" s="7"/>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>94</v>
@@ -2074,16 +2097,16 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>61</v>
@@ -2099,28 +2122,28 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F24" t="s">
         <v>47</v>
@@ -2129,16 +2152,16 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>23</v>
@@ -2160,7 +2183,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28">
+    <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>19</v>
       </c>
@@ -2177,16 +2210,13 @@
         <v>88</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15">
-      <c r="A27" s="6" t="s">
-        <v>176</v>
-      </c>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="s">
         <v>21</v>
       </c>
@@ -2203,22 +2233,15 @@
         <v>86</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3" t="s">
-        <v>25</v>
+    <row r="28" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
@@ -2240,18 +2263,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>178</v>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3</v>
@@ -2273,18 +2294,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="20" t="s">
-        <v>184</v>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>186</v>
+        <v>114</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>4</v>
@@ -2306,18 +2327,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="11" t="s">
-        <v>61</v>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>182</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>60</v>
+        <v>203</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>5</v>
@@ -2339,7 +2360,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="F32" s="1" t="s">
         <v>93</v>
       </c>
@@ -2348,20 +2381,17 @@
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>101</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="15">
-      <c r="A33" s="6" t="s">
-        <v>133</v>
-      </c>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J33" s="1" t="s">
         <v>22</v>
       </c>
@@ -2373,670 +2403,677 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="16" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" s="1" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="15">
-      <c r="A38" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="3" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="11" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="13" t="s">
-        <v>179</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="1"/>
+      <c r="C42" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="D42" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15">
-      <c r="A47" s="6" t="s">
+    <row r="48" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="3" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="28">
-      <c r="A49" s="10" t="s">
+    <row r="50" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>7</v>
+        <v>153</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>101</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B59" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B60" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1" t="s">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15">
-      <c r="A62" s="6" t="s">
+    <row r="63" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="3" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3" t="s">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" s="1" t="s">
+    <row r="71" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A71" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="C72" s="4"/>
+      <c r="D72" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15">
-      <c r="A68" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="28">
-      <c r="A70" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15">
-      <c r="A73" s="6" t="s">
+      <c r="C76" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B73" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D75" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="1" t="s">
-        <v>2</v>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="D77" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15">
-      <c r="A82" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B82" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B83" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3" t="s">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="11" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D84" s="1" t="s">
+      <c r="C85" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="B85" s="1" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B86" s="4" t="s">
+      <c r="C86" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15">
-      <c r="A88" s="6" t="s">
+      <c r="C87" s="4"/>
+      <c r="D87" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A89" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="3" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3" t="s">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="11" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D90" s="1" t="s">
+      <c r="C91" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="8" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15">
-      <c r="A94" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="3" t="s">
+    <row r="95" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A95" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3" t="s">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="1" t="s">
-        <v>13</v>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C97" s="1"/>
+      <c r="C97" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="D97" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3044,7 +3081,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3061,34 +3098,34 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:4" ht="28">
+    <row r="2" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -3100,7 +3137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -3112,7 +3149,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3124,7 +3161,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -3136,43 +3173,43 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -3184,7 +3221,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -3196,7 +3233,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>61</v>
       </c>
@@ -3204,13 +3241,13 @@
         <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>74</v>
       </c>
@@ -3218,13 +3255,13 @@
         <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>75</v>
       </c>
@@ -3236,9 +3273,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>101</v>
@@ -3246,9 +3283,9 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>101</v>
@@ -3256,17 +3293,17 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Parallel logic by thread for SourceFileVectorCreator, ScmRepoAnalyzer, StackTraceAnalyzer, BLIA, Evaluator to improve performance.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="229">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -857,83 +857,93 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>UNIQUE COMP_IDX_BUG_SF_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALPHA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BETA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAST_DAYS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP1_RATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP5_RATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP10_RATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top 1 ranked rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top 5 ranked rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top 10 ranked rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tables for BLIA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDX_SF_INFO_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLS_NAME(Unique)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE IDX_SF_INFO_CLS_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_INFO_PROD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_BUG_INFO_FDATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_TERM_WGT,
+IDX_BUG_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_SF_TERM_WGT
+IDX_BUG_SF_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>UNIQUE COMP_IDX_BUG_TERM_WGT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>UNIQUE COMP_IDX_BUG_SF_TERM_WGT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>BUG_TERM_WGT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALPHA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BETA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAST_DAYS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TOP1_RATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TOP5_RATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TOP10_RATE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top 1 ranked rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top 5 ranked rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top 10 ranked rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tables for BLIA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE IDX_SF_INFO_NAME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CLS_NAME(Unique)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNIQUE IDX_SF_INFO_CLS_NAME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Class name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_BUG_INFO_PROD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_BUG_INFO_FDATE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1542,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1564,7 +1574,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1684,7 +1694,7 @@
         <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>29</v>
@@ -1713,16 +1723,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>61</v>
@@ -2581,7 +2591,7 @@
         <v>88</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>60</v>
@@ -2607,7 +2617,7 @@
         <v>102</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>50</v>
@@ -2831,15 +2841,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>208</v>
+      <c r="C76" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>49</v>
@@ -2853,7 +2863,7 @@
         <v>86</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>176</v>
@@ -2909,7 +2919,7 @@
     </row>
     <row r="83" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="B83" t="s">
         <v>124</v>
@@ -2927,15 +2937,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>207</v>
+      <c r="C85" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>49</v>
@@ -2949,7 +2959,7 @@
         <v>86</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>180</v>
@@ -3175,38 +3185,38 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3275,7 +3285,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>101</v>
@@ -3285,7 +3295,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>101</v>
@@ -3295,10 +3305,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>

</xml_diff>

<commit_message>
DB schema changed(data type of BUG_ID changed from string to int). Non-thread mode of BLIA class. Property.LIMIT_CANDIDATE_SIZE added to limit calculation of analysis. BugDAO.insertStructuredBug() added. SourceFileDAO.insertStructuredCorpusSet() added. Missed BUG_INFO.FIXED_DATE index added. EvaluatorTest's step is seperated(prepareAnalysisData, preAnalyze, anlayze)
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="14505"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20280" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis DB" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="231">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -115,10 +115,6 @@
   </si>
   <si>
     <t>FUNC_COR_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BLIA_SCORE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -280,11 +276,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Bug ID
-ex.) BLIA-10234</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Code change ID
 ex.) BLIA-8732</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -944,6 +935,24 @@
   </si>
   <si>
     <t>BUG_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug ID
+ex.) 10234</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_INT_ANAL_BLIA_SCORE
+DESC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BLIA_SCORE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1182,7 +1191,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1254,6 +1263,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1552,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1574,7 +1586,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1607,48 +1619,48 @@
     </row>
     <row r="3" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="J4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="33" x14ac:dyDescent="0.3">
@@ -1656,210 +1668,210 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="33" x14ac:dyDescent="0.3">
@@ -1867,213 +1879,213 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="J14" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="J15" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="J19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2081,51 +2093,51 @@
         <v>1</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -2134,96 +2146,96 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="J25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -2231,249 +2243,250 @@
         <v>21</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="L30" s="4"/>
+        <v>99</v>
+      </c>
       <c r="M30" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J33" s="1" t="s">
-        <v>22</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="J33" s="14" t="s">
+        <v>230</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="L33" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="L33" s="24" t="s">
+        <v>229</v>
+      </c>
       <c r="M33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -2481,27 +2494,27 @@
         <v>16</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -2509,11 +2522,11 @@
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -2521,11 +2534,11 @@
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -2533,11 +2546,11 @@
         <v>4</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -2545,28 +2558,28 @@
         <v>5</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -2574,271 +2587,271 @@
         <v>8</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>62</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>62</v>
+        <v>228</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
@@ -2846,27 +2859,27 @@
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2874,11 +2887,11 @@
         <v>2</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2886,11 +2899,11 @@
         <v>3</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2898,11 +2911,11 @@
         <v>4</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2910,31 +2923,31 @@
         <v>5</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
@@ -2942,56 +2955,56 @@
         <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2999,68 +3012,68 @@
         <v>6</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -3068,11 +3081,11 @@
         <v>13</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -3080,7 +3093,7 @@
         <v>12</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -3118,7 +3131,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -3132,197 +3145,197 @@
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
candidateLimitRate, candidateLimitSize added to reduce anlaysis computing time Evaluator's thread error of synchronization fixed
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20280" windowHeight="6840"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20280" windowHeight="6840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis DB" sheetId="1" r:id="rId1"/>
@@ -1258,14 +1258,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1564,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1585,21 +1585,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
@@ -2419,7 +2419,7 @@
       <c r="K33" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="L33" s="24" t="s">
+      <c r="L33" s="22" t="s">
         <v>229</v>
       </c>
       <c r="M33" s="1" t="s">
@@ -3117,8 +3117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3130,12 +3130,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
@@ -3234,26 +3234,26 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1. Because experiment results of AspectJ were wrong, file path handling logic fixed again. master branch is also fixed. Refer to BLIA v0.8.7 version. 2. Extended bug repository with comments for each bug report. 3. Comment class added. 4. Added BLIA+ algorithm name. 5. Comment table is added to DB schema.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,34 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaus\Dropbox\Workspace\BLIA\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Klaus/git/BLIA/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20280" windowHeight="6840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis DB" sheetId="1" r:id="rId1"/>
     <sheet name="Evaluation DB" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="242">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -954,13 +954,46 @@
   <si>
     <t>BLIA_SCORE</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_CMT_INFO</t>
+  </si>
+  <si>
+    <t>CMT_ID</t>
+  </si>
+  <si>
+    <t>ATHR</t>
+  </si>
+  <si>
+    <t>Comment ID</t>
+  </si>
+  <si>
+    <t>CMT_COR</t>
+  </si>
+  <si>
+    <t>Comment corpus</t>
+  </si>
+  <si>
+    <t>Author information</t>
+  </si>
+  <si>
+    <t>CMT_DATE</t>
+  </si>
+  <si>
+    <t>Commeted date</t>
+  </si>
+  <si>
+    <t>IDX_BUG_CMT_INFO</t>
+  </si>
+  <si>
+    <t>Similarity between previous report and current one.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1063,6 +1096,12 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="맑은 고딕"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1143,7 +1182,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1190,8 +1229,260 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1255,12 +1546,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="12" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="12" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1268,23 +1568,107 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="16">
-    <cellStyle name="40% - 강조색2" xfId="12" builtinId="35"/>
-    <cellStyle name="강조색2" xfId="11" builtinId="33"/>
-    <cellStyle name="메모" xfId="15" builtinId="10"/>
-    <cellStyle name="보통" xfId="1" builtinId="28"/>
+  <cellStyles count="100">
+    <cellStyle name="40% - 강조2" xfId="12" builtinId="35"/>
+    <cellStyle name="강조2" xfId="11" builtinId="33"/>
+    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="노트" xfId="15" builtinId="10"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="좋음" xfId="6" builtinId="26"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="중간" xfId="1" builtinId="28"/>
     <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="하이퍼링크" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="98" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1562,46 +1946,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.125" customWidth="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1"/>
-    <col min="6" max="6" width="21.125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" customWidth="1"/>
-    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-    </row>
-    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+    </row>
+    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1617,7 +2002,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -1628,7 +2013,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1663,7 +2048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="34" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1698,7 +2083,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>98</v>
       </c>
@@ -1733,7 +2118,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>218</v>
       </c>
@@ -1766,7 +2151,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>60</v>
       </c>
@@ -1790,7 +2175,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>44</v>
       </c>
@@ -1805,7 +2190,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
@@ -1819,7 +2204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1843,7 +2228,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>88</v>
       </c>
@@ -1874,7 +2259,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
@@ -1909,7 +2294,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>89</v>
       </c>
@@ -1942,7 +2327,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>156</v>
       </c>
@@ -1973,7 +2358,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>157</v>
       </c>
@@ -1994,7 +2379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>158</v>
       </c>
@@ -2006,7 +2391,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>159</v>
       </c>
@@ -2024,7 +2409,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
@@ -2055,7 +2440,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>107</v>
       </c>
@@ -2088,11 +2473,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C21" s="7"/>
@@ -2119,11 +2504,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C22" s="4"/>
@@ -2144,11 +2529,11 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C23" s="4"/>
@@ -2156,11 +2541,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C24" s="4"/>
@@ -2174,11 +2559,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C25" s="4"/>
@@ -2205,11 +2590,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C26" s="4"/>
@@ -2238,7 +2623,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F27" s="1" t="s">
         <v>21</v>
       </c>
@@ -2261,7 +2646,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>172</v>
       </c>
@@ -2285,7 +2670,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -2316,7 +2701,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>173</v>
       </c>
@@ -2348,7 +2733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>180</v>
       </c>
@@ -2381,7 +2766,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>60</v>
       </c>
@@ -2412,26 +2797,26 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="34" x14ac:dyDescent="0.25">
       <c r="J33" s="14" t="s">
         <v>230</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="L33" s="22" t="s">
+      <c r="L33" s="21" t="s">
         <v>229</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
@@ -2443,7 +2828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>88</v>
       </c>
@@ -2457,7 +2842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>130</v>
       </c>
@@ -2469,7 +2854,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>202</v>
       </c>
@@ -2477,7 +2862,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
@@ -2489,7 +2874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>16</v>
       </c>
@@ -2503,7 +2888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>175</v>
       </c>
@@ -2517,7 +2902,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>2</v>
       </c>
@@ -2529,7 +2914,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -2541,7 +2926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -2553,7 +2938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
@@ -2565,12 +2950,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
@@ -2582,7 +2967,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>8</v>
       </c>
@@ -2596,7 +2981,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>60</v>
       </c>
@@ -2610,7 +2995,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>151</v>
       </c>
@@ -2622,7 +3007,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>7</v>
       </c>
@@ -2636,7 +3021,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>166</v>
       </c>
@@ -2648,7 +3033,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>167</v>
       </c>
@@ -2660,7 +3045,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>168</v>
       </c>
@@ -2672,7 +3057,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>107</v>
       </c>
@@ -2684,11 +3069,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C58" s="4"/>
@@ -2696,11 +3081,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C59" s="4"/>
@@ -2708,11 +3093,11 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C60" s="4"/>
@@ -2720,7 +3105,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>135</v>
       </c>
@@ -2732,12 +3117,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="22"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>22</v>
       </c>
@@ -2749,354 +3143,435 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="s">
+    <row r="65" spans="1:4" ht="34" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="13" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+    <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3" t="s">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A71" s="16" t="s">
+    <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="15" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4" t="s">
+      <c r="C80" s="4"/>
+      <c r="D80" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+    <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B82" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3" t="s">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="11" t="s">
+    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="B83" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A85" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="13" t="s">
-        <v>181</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C88" s="4"/>
+      <c r="D88" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89" s="4"/>
+      <c r="D89" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B91" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4" t="s">
+      <c r="C95" s="4"/>
+      <c r="D95" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
+    <row r="97" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B98" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3" t="s">
+      <c r="C98" s="3"/>
+      <c r="D98" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="11" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="8" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1" t="s">
+      <c r="C100" s="1"/>
+      <c r="D100" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="9" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1" t="s">
+      <c r="C101" s="1"/>
+      <c r="D101" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
+    <row r="103" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3" t="s">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="12" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1" t="s">
+      <c r="C106" s="1"/>
+      <c r="D106" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1" t="s">
+        <v>241</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3104,12 +3579,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" scale="39" orientation="portrait"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 
@@ -3117,38 +3590,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-    </row>
-    <row r="2" spans="1:4" ht="33.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -3160,7 +3633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
@@ -3172,7 +3645,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -3184,7 +3657,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>71</v>
       </c>
@@ -3196,7 +3669,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>209</v>
       </c>
@@ -3208,7 +3681,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>210</v>
       </c>
@@ -3220,7 +3693,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>211</v>
       </c>
@@ -3232,7 +3705,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
@@ -3244,7 +3717,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -3256,7 +3729,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>60</v>
       </c>
@@ -3270,7 +3743,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>72</v>
       </c>
@@ -3284,7 +3757,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
@@ -3296,7 +3769,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>206</v>
       </c>
@@ -3306,7 +3779,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>207</v>
       </c>
@@ -3316,7 +3789,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>208</v>
       </c>
@@ -3326,7 +3799,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -3344,10 +3817,5 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tables added and extended to method level's bug localization
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680"/>
+    <workbookView xWindow="-1800" yWindow="-17540" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis DB" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="257">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -90,31 +90,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>FUNC_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SF_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_NAME(Unique)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_COR_ID(KEY)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_COR_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -187,36 +163,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Function ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Function name
-ex.) edu.skku.selab.blia.blia.main</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Function &amp; version relation ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Corpus from function</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_VER_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_COR_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FUNC_ANALYSIS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -437,10 +384,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>FIXED_FUNC_VER_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>COMM_DATE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -987,13 +930,119 @@
   </si>
   <si>
     <t>Similarity between previous report and current one.</t>
+  </si>
+  <si>
+    <t>COMM_MTH_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_COMM_MTH_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_MTH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commited method name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_ID(KEY)</t>
+  </si>
+  <si>
+    <t>MTH_NAME(Unique)</t>
+  </si>
+  <si>
+    <t>UNIQUE IDX_MTH_INFO_NAME</t>
+  </si>
+  <si>
+    <t>MTH_VER_INFO</t>
+  </si>
+  <si>
+    <t>MTH_VER_ID</t>
+  </si>
+  <si>
+    <t>MTH_ID</t>
+  </si>
+  <si>
+    <t>MTH_COR_INFO</t>
+  </si>
+  <si>
+    <t>MTH_COR_ID(KEY)</t>
+  </si>
+  <si>
+    <t>MTH_ANALYSIS</t>
+  </si>
+  <si>
+    <t>MTH_COR_ID</t>
+  </si>
+  <si>
+    <t>FIXED_MTH_VER_ID</t>
+  </si>
+  <si>
+    <t>Method ID</t>
+  </si>
+  <si>
+    <t>Method ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method name
+ex.) edu.skku.selab.blia.blia.main</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method &amp; version relation ID</t>
+  </si>
+  <si>
+    <t>INT_MTH_ANALYSIS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BLIA_MTH_SCORE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_INT_MTH_ANAL_BUG_ID,
+UNIQUE COMP_IDX_INT_MTH_ANALSYS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_INT_MTH_ANALSYS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_INT_MTH_ANAL_BLIA_MTH_SCORE
+DESC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1102,8 +1151,16 @@
       <name val="맑은 고딕"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1140,6 +1197,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1482,7 +1545,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1510,9 +1573,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="11" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1566,6 +1626,27 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="100">
@@ -1946,1413 +2027,1573 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N107"/>
+  <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="8" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-    </row>
-    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="19"/>
-    </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="32" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+    </row>
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="34" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="68" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F6" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="34" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
+    </row>
+    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>88</v>
+        <v>18</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="K11" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>22</v>
+      <c r="F12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="34" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>148</v>
+        <v>20</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>89</v>
+        <v>134</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>144</v>
+        <v>25</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29" t="s">
+        <v>246</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K15" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F15" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="34" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="K19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>90</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
       <c r="K20" s="1" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>63</v>
+        <v>27</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F24" t="s">
+        <v>179</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="F27" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L28" s="4"/>
-      <c r="M28" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F31" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L29" s="4"/>
-      <c r="M29" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="G31" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="G32" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="F33" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="G33" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L32" s="4"/>
-      <c r="M32" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="34" x14ac:dyDescent="0.25">
-      <c r="J33" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="H33" s="30"/>
+      <c r="I33" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="29"/>
+      <c r="K34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
-        <v>88</v>
+        <v>18</v>
+      </c>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="K35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>130</v>
+        <v>20</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M38" s="4"/>
+      <c r="N38" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M40" s="4"/>
+      <c r="N40" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="34" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>175</v>
+      <c r="K41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M41" s="4"/>
+      <c r="N41" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="34" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>161</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M42" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="K45" s="32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="51" x14ac:dyDescent="0.25">
+      <c r="K47" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M49" s="4"/>
+      <c r="N49" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="51" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>60</v>
+        <v>214</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M50" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C65" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>228</v>
+      <c r="A65" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C66" s="23"/>
-      <c r="D66" s="23" t="s">
-        <v>234</v>
+      <c r="A66" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23" t="s">
-        <v>237</v>
+      <c r="A67" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="23"/>
-      <c r="D68" s="23" t="s">
-        <v>239</v>
+      <c r="A68" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C69" s="23"/>
-      <c r="D69" s="23" t="s">
-        <v>236</v>
+      <c r="A69" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
-        <v>177</v>
+      <c r="A73" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="s">
-        <v>180</v>
+      <c r="A74" s="12" t="s">
+        <v>166</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
-        <v>121</v>
+      <c r="A75" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
-        <v>126</v>
+      <c r="A79" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="15" t="s">
-        <v>133</v>
+      <c r="A80" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B82" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="68" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
-        <v>175</v>
+      <c r="A85" s="12" t="s">
+        <v>161</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3360,11 +3601,11 @@
         <v>2</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3372,11 +3613,11 @@
         <v>3</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3384,11 +3625,11 @@
         <v>4</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,157 +3637,157 @@
         <v>5</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B91" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="68" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="s">
-        <v>181</v>
+      <c r="A94" s="12" t="s">
+        <v>167</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
+      <c r="A99" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
-        <v>102</v>
+      <c r="A101" s="31" t="s">
+        <v>245</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>39</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>114</v>
+      <c r="A105" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,11 +3795,11 @@
         <v>13</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,22 +3807,22 @@
         <v>12</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" orientation="portrait"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="13" max="1048575" man="1"/>
+    <brk id="14" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
@@ -3603,212 +3844,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="A1" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>60</v>
+      <c r="A13" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Overall modules are extended for extended bug repository and commit information. ExtendedZXingBugRepository.xml added. MethodVisitor class moved to common package. MethodTest added.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="249">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1007,6 +1007,14 @@
   </si>
   <si>
     <t>Commited method info(method name|return type|parameters)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_MTH_HASH_KEY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hash key value of commited method</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1960,8 +1968,8 @@
   </sheetPr>
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1971,7 +1979,7 @@
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.5" bestFit="1" customWidth="1"/>
@@ -2366,6 +2374,16 @@
       <c r="D21" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -2379,7 +2397,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>159</v>
       </c>
@@ -2390,11 +2408,8 @@
       <c r="D23" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>161</v>
       </c>
@@ -2405,15 +2420,8 @@
       <c r="D24" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3" t="s">
-        <v>18</v>
+      <c r="F24" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2427,39 +2435,45 @@
       <c r="D25" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="F27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -2472,8 +2486,12 @@
       <c r="D28" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>145</v>
       </c>
@@ -2486,11 +2504,8 @@
       <c r="D29" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>152</v>
       </c>
@@ -2503,46 +2518,37 @@
       <c r="D30" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3" t="s">
+      <c r="H31" s="3"/>
+      <c r="I31" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="F31" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="13" t="s">
-        <v>82</v>
+      <c r="F32" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>98</v>
+      <c r="H32" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2556,15 +2562,17 @@
       <c r="D33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="4"/>
+      <c r="F33" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="I33" s="1" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2581,14 +2589,14 @@
         <v>20</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>78</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2603,25 +2611,25 @@
         <v>101</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="H35" s="4"/>
       <c r="I35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F36" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H36" s="4"/>
       <c r="I36" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -2632,17 +2640,17 @@
         <v>96</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>78</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="34" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
@@ -2653,17 +2661,15 @@
       <c r="D38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="13" t="s">
-        <v>200</v>
+      <c r="F38" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H38" s="20" t="s">
-        <v>199</v>
-      </c>
+      <c r="H38" s="4"/>
       <c r="I38" s="1" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="34" x14ac:dyDescent="0.25">
@@ -2679,6 +2685,18 @@
       <c r="D39" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F39" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -2694,7 +2712,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -2705,11 +2723,8 @@
       <c r="D41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -2720,18 +2735,11 @@
       <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="F42" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -2742,20 +2750,18 @@
       <c r="D43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -2766,48 +2772,60 @@
       <c r="D44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="F44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F45" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F45" s="1" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H45" s="4"/>
-      <c r="I45" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="F46" s="13" t="s">
-        <v>219</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H46" s="20" t="s">
-        <v>223</v>
-      </c>
+      <c r="H46" s="4"/>
       <c r="I46" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>236</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Basically method level's bug localization logic and evaluation method was implemented. ExtendedAspectJBugRepository.xml, ExtendedSWTBugRepository.xml were added and their XML syntax was verified. IntegratedMethodAnalysisValue renamed to ExtendedIntegratedAnalysisValue
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="250">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -921,10 +921,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>MTH_NAME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>RET_TYPE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1015,6 +1011,14 @@
   </si>
   <si>
     <t>Hash key value of commited method</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_MTH_INFO_NAME</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1968,8 +1972,8 @@
   </sheetPr>
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2274,7 @@
         <v>135</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2353,14 +2357,14 @@
         <v>25</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2375,14 +2379,14 @@
         <v>162</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2813,7 +2817,7 @@
     </row>
     <row r="47" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F47" s="13" t="s">
         <v>219</v>
@@ -2858,66 +2862,68 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>225</v>
+      <c r="A51" s="12" t="s">
+        <v>248</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C51" s="1"/>
+        <v>226</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3419,7 +3425,7 @@
     </row>
     <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3442,7 +3448,7 @@
         <v>66</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>31</v>
@@ -3462,7 +3468,7 @@
     </row>
     <row r="109" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3485,7 +3491,7 @@
         <v>66</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>31</v>
@@ -3493,7 +3499,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
MethodAnalyzer was newly added to extend BLIA's method level bug localization
Inner classes' methods included to analyze source file contents
DB tables were extended for MethodAnalyzer
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="256">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -332,10 +332,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>COMM_FILE_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>COMM_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -393,10 +389,6 @@
   </si>
   <si>
     <t>IDX_SIMI_BUG_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDX_COMM_FILE_INFO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -496,10 +488,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>COMM_FILE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>VARCHAR(255)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -827,15 +815,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>IDX_INT_ANAL_BLIA_SCORE
-DESC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BLIA_SCORE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>BUG_CMT_INFO</t>
   </si>
   <si>
@@ -1019,6 +998,52 @@
   </si>
   <si>
     <t>IDX_MTH_INFO_NAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_SF_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_SF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMM_SF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BLIA_SF_SCORE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MID_SF_SCORE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_INT_ANAL_MID_SF_SCORE
+DESC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_INT_ANAL_BLIA_SF_SCORE
+DESC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File level's BLIA score</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method level's BLIA score</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VSM score of method</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_COMM_SF_INFO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1509,7 +1534,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1570,9 +1595,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="12" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1581,6 +1603,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1972,8 +2009,8 @@
   </sheetPr>
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1990,17 +2027,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="A1" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
@@ -2030,7 +2067,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>18</v>
@@ -2042,7 +2079,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>18</v>
@@ -2056,7 +2093,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>20</v>
@@ -2065,10 +2102,10 @@
         <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>43</v>
@@ -2076,22 +2113,22 @@
     </row>
     <row r="6" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
@@ -2100,38 +2137,38 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -2151,7 +2188,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>75</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2162,7 +2199,7 @@
         <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>23</v>
@@ -2186,21 +2223,21 @@
         <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I12" s="2" t="s">
+      <c r="F12" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="I12" s="22" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2212,81 +2249,81 @@
         <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1" t="s">
-        <v>119</v>
+      <c r="F13" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="4" t="s">
-        <v>112</v>
+        <v>130</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>16</v>
@@ -2301,23 +2338,23 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>76</v>
+        <v>134</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>43</v>
@@ -2325,24 +2362,24 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>117</v>
+        <v>168</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2350,79 +2387,79 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>244</v>
+      <c r="F20" s="8" t="s">
+        <v>239</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>46</v>
@@ -2430,14 +2467,14 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>16</v>
@@ -2458,7 +2495,7 @@
         <v>69</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>47</v>
@@ -2466,13 +2503,13 @@
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
@@ -2497,30 +2534,30 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>34</v>
@@ -2540,7 +2577,7 @@
     </row>
     <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>6</v>
@@ -2549,7 +2586,7 @@
         <v>66</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>31</v>
@@ -2567,16 +2604,16 @@
         <v>18</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>66</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2587,7 +2624,7 @@
         <v>66</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>20</v>
@@ -2596,7 +2633,7 @@
         <v>11</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="1" t="s">
@@ -2605,20 +2642,20 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="1" t="s">
@@ -2630,7 +2667,7 @@
         <v>14</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>37</v>
@@ -2638,18 +2675,18 @@
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
-      </c>
-      <c r="F37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H37" s="4"/>
+      <c r="G37" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="25"/>
       <c r="I37" s="1" t="s">
         <v>39</v>
       </c>
@@ -2665,15 +2702,15 @@
       <c r="D38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H38" s="4"/>
+      <c r="F38" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="25"/>
       <c r="I38" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="34" x14ac:dyDescent="0.25">
@@ -2684,19 +2721,19 @@
         <v>66</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F39" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>199</v>
+      <c r="F39" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="26" t="s">
+        <v>250</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>40</v>
@@ -2704,16 +2741,28 @@
     </row>
     <row r="40" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H40" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2728,7 +2777,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -2739,97 +2788,75 @@
       <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="F46" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="I44" s="1" t="s">
+      <c r="H46" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F45" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="G45" s="4" t="s">
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="G47" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F46" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H47" s="20" t="s">
-        <v>223</v>
+      <c r="H47" s="27" t="s">
+        <v>216</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>40</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2840,110 +2867,142 @@
         <v>17</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F48" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H48" s="25"/>
+      <c r="I48" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H49" s="25"/>
+      <c r="I49" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="34" x14ac:dyDescent="0.25">
+      <c r="F50" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>16</v>
       </c>
@@ -2955,133 +3014,133 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>69</v>
@@ -3092,14 +3151,14 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
+      <c r="A70" s="20"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -3118,70 +3177,70 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="s">
-        <v>90</v>
+      <c r="A73" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D73" s="23" t="s">
-        <v>198</v>
+        <v>205</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
-        <v>202</v>
+      <c r="A74" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3198,35 +3257,35 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3243,36 +3302,36 @@
     </row>
     <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B89" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3292,10 +3351,10 @@
         <v>6</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>31</v>
@@ -3303,16 +3362,16 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3344,7 +3403,7 @@
         <v>4</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="1" t="s">
@@ -3356,7 +3415,7 @@
         <v>5</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C96" s="4"/>
       <c r="D96" s="1" t="s">
@@ -3365,10 +3424,10 @@
     </row>
     <row r="98" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B98" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3388,10 +3447,10 @@
         <v>6</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>31</v>
@@ -3399,33 +3458,33 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C102" s="4"/>
       <c r="D102" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3448,7 +3507,7 @@
         <v>66</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>31</v>
@@ -3456,7 +3515,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>66</v>
@@ -3468,7 +3527,7 @@
     </row>
     <row r="109" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3491,7 +3550,7 @@
         <v>66</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>31</v>
@@ -3499,19 +3558,19 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3528,13 +3587,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>31</v>
@@ -3557,11 +3616,11 @@
         <v>12</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3594,12 +3653,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="A1" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
@@ -3662,38 +3721,38 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3701,7 +3760,7 @@
         <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
@@ -3713,7 +3772,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
@@ -3728,7 +3787,7 @@
         <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>41</v>
@@ -3742,7 +3801,7 @@
         <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>63</v>
@@ -3762,30 +3821,30 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -3795,7 +3854,7 @@
         <v>56</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">

</xml_diff>

<commit_message>
MethodVsmScore calculation logic fixed. RUN_LEVEL property is added. (FILE or METHOD) BugMethodVectorCreator added to anlayze method vector. BugDAO's minor query error fixed.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="265">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1044,6 +1044,43 @@
   </si>
   <si>
     <t>IDX_COMM_SF_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_MTH_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_SF_TERM_WGT
+IDX_BUG_MTH_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNIQUE COMP_IDX_BUG_MTH_TERM_WGT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_TERM_ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method term ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug ID에서 추출한 파일들에서 나온 Methods의 corpus 간의 분석, Bug report의 corpus에 대한 Methods의 vector값을 찾아냄.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_NORM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>norm of methods in ranked suspicious files</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTH_TOT_CNT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1155,7 +1192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1192,6 +1229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1534,7 +1577,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1624,6 +1667,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="100">
@@ -2007,10 +2053,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -3139,487 +3185,591 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1" t="s">
+      <c r="C71" s="1"/>
+      <c r="D71" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-    </row>
-    <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3" t="s">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A73" s="21" t="s">
+    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C75" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D75" s="22" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="21" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B76" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3" t="s">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3" t="s">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A86" s="15" t="s">
+    <row r="88" spans="1:9" ht="34" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4" t="s">
+      <c r="C89" s="4"/>
+      <c r="D89" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B91" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+      <c r="F91" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="G91" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3" t="s">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="68" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+      <c r="F92" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="68" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="12" t="s">
+      <c r="F93" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C94" s="1"/>
+      <c r="C94" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="D94" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F94" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="F96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C95" s="4"/>
-      <c r="D95" s="1" t="s">
+      <c r="C97" s="4"/>
+      <c r="D97" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="F97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H97" s="4"/>
+      <c r="I97" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C96" s="4"/>
-      <c r="D96" s="1" t="s">
+      <c r="C98" s="4"/>
+      <c r="D98" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
+      <c r="F98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H98" s="4"/>
+      <c r="I98" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3" t="s">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="68" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
+    <row r="102" spans="1:9" ht="68" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="12" t="s">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4" t="s">
+      <c r="C104" s="4"/>
+      <c r="D104" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
+    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3" t="s">
+      <c r="C107" s="3"/>
+      <c r="D107" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1" t="s">
+      <c r="C109" s="1"/>
+      <c r="D109" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A109" s="6" t="s">
+    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3" t="s">
+      <c r="C112" s="3"/>
+      <c r="D112" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1" t="s">
+      <c r="C114" s="1"/>
+      <c r="D114" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A114" s="6" t="s">
+    <row r="116" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A116" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3" t="s">
+      <c r="C117" s="3"/>
+      <c r="D117" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="11" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1" t="s">
+      <c r="C119" s="1"/>
+      <c r="D119" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1" t="s">
+      <c r="C120" s="1"/>
+      <c r="D120" s="1" t="s">
         <v>206</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added gamma value for bug localization on the method level. Related ExperimentResultDAO and classes were extended.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -957,10 +957,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>BUG_FIX_SF_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>IDX_BUG_FIX_SF_INFO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1081,6 +1077,10 @@
   </si>
   <si>
     <t>MTH_TOT_CNT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUG_FIX_SF_INFO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1192,7 +1192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1229,12 +1229,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1577,7 +1571,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1667,9 +1661,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="100">
@@ -2055,8 +2046,8 @@
   </sheetPr>
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2234,7 +2225,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2281,7 +2272,7 @@
         <v>118</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I12" s="22" t="s">
         <v>43</v>
@@ -2301,7 +2292,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>115</v>
@@ -2418,7 +2409,7 @@
         <v>168</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>67</v>
@@ -2440,14 +2431,14 @@
         <v>25</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2462,14 +2453,14 @@
         <v>159</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>225</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2773,13 +2764,13 @@
         <v>23</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G39" s="25" t="s">
         <v>77</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>40</v>
@@ -2799,16 +2790,16 @@
         <v>143</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G40" s="25" t="s">
         <v>77</v>
       </c>
       <c r="H40" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2926,7 +2917,7 @@
       </c>
       <c r="H48" s="25"/>
       <c r="I48" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2976,18 +2967,18 @@
         <v>218</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>227</v>
@@ -3007,14 +2998,14 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3185,8 +3176,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="s">
-        <v>264</v>
+      <c r="A69" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>85</v>
@@ -3197,15 +3188,15 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="30" t="s">
-        <v>262</v>
+      <c r="A70" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,10 +3395,10 @@
         <v>123</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G91" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3452,7 +3443,7 @@
         <v>194</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>31</v>
@@ -3472,16 +3463,16 @@
         <v>143</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>66</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3634,7 +3625,7 @@
     </row>
     <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -3657,7 +3648,7 @@
         <v>66</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>31</v>
@@ -3677,7 +3668,7 @@
     </row>
     <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed filtering date from fixed date to open date of new bug report while analyzing similarity among bug reports 1. BUG_INFO.CMT_COR column added. 2. filtering date changed(fixed date => open date) 3. Comment excluded when calculating cosine similarity among bug reports.
</commit_message>
<xml_diff>
--- a/doc/DB schema design.xlsx
+++ b/doc/DB schema design.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="267">
   <si>
     <t>SF_ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -576,10 +579,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DESC_COR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Summary corpus</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1081,6 +1080,18 @@
   </si>
   <si>
     <t>BUG_FIX_SF_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DESC_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMT_COR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment corpus</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2044,10 +2055,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2065,7 +2076,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -2156,7 +2167,7 @@
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
@@ -2174,16 +2185,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>108</v>
@@ -2225,7 +2236,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2272,7 +2283,7 @@
         <v>118</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I12" s="22" t="s">
         <v>43</v>
@@ -2292,7 +2303,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>115</v>
@@ -2348,7 +2359,7 @@
         <v>132</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2391,7 +2402,7 @@
         <v>118</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>43</v>
@@ -2406,10 +2417,10 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>67</v>
@@ -2431,72 +2442,72 @@
         <v>25</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>46</v>
@@ -2504,14 +2515,14 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>16</v>
@@ -2540,7 +2551,7 @@
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>45</v>
@@ -2571,7 +2582,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>66</v>
@@ -2580,21 +2591,21 @@
         <v>88</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>34</v>
@@ -2712,7 +2723,7 @@
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B37" t="s">
         <v>94</v>
@@ -2758,19 +2769,19 @@
         <v>66</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G39" s="25" t="s">
         <v>77</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>40</v>
@@ -2778,28 +2789,28 @@
     </row>
     <row r="40" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G40" s="25" t="s">
         <v>77</v>
       </c>
       <c r="H40" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2850,7 +2861,7 @@
         <v>29</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2873,7 +2884,7 @@
         <v>66</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>31</v>
@@ -2881,19 +2892,19 @@
     </row>
     <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G47" s="25" t="s">
         <v>66</v>
       </c>
       <c r="H47" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2904,7 +2915,7 @@
         <v>17</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>18</v>
@@ -2917,21 +2928,21 @@
       </c>
       <c r="H48" s="25"/>
       <c r="I48" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F49" s="27" t="s">
         <v>120</v>
@@ -2946,80 +2957,80 @@
     </row>
     <row r="50" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G50" s="25" t="s">
         <v>77</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="34" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3056,13 +3067,13 @@
         <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3085,7 +3096,7 @@
         <v>78</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>32</v>
@@ -3112,656 +3123,668 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>137</v>
+        <v>264</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4" t="s">
-        <v>168</v>
+        <v>265</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>263</v>
+        <v>164</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>262</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1" t="s">
+      <c r="C72" s="1"/>
+      <c r="D72" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-    </row>
-    <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
-        <v>196</v>
-      </c>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="20"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3" t="s">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.25">
-      <c r="A75" s="21" t="s">
+    <row r="76" spans="1:4" ht="34" x14ac:dyDescent="0.25">
+      <c r="A76" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="21" t="s">
-        <v>197</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8" t="s">
-        <v>199</v>
+      <c r="C76" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>198</v>
+      <c r="A77" s="21" t="s">
+        <v>196</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="8" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="B84" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B84" s="1" t="s">
+    <row r="89" spans="1:9" ht="34" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="C90" s="4"/>
+      <c r="D90" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B92" t="s">
+        <v>123</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="G92" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3" t="s">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="34" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B91" t="s">
-        <v>123</v>
-      </c>
-      <c r="F91" s="6" t="s">
+      <c r="F93" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="68" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H94" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G91" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H92" s="3"/>
-      <c r="I92" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="68" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D93" s="1" t="s">
+      <c r="I94" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F93" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D94" s="1" t="s">
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="F94" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C95" s="1"/>
+      <c r="C95" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="D95" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>2</v>
+        <v>142</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>257</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H95" s="1"/>
+      <c r="H95" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="I95" s="1" t="s">
-        <v>26</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>66</v>
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C97" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G97" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H97" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H97" s="1"/>
       <c r="I97" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H98" s="4"/>
       <c r="I98" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C99" s="4"/>
+      <c r="D99" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
+      <c r="F99" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H99" s="4"/>
+      <c r="I99" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B101" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="68" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B100" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="C103" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3" t="s">
+      <c r="C108" s="3"/>
+      <c r="D108" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="68" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A106" s="6" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C109" s="1"/>
+      <c r="C109" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="D109" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3" t="s">
+      <c r="C113" s="3"/>
+      <c r="D113" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="10" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C114" s="1"/>
+      <c r="C114" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="D114" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A116" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3" t="s">
+      <c r="C118" s="3"/>
+      <c r="D118" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="11" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C119" s="1"/>
+      <c r="C119" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D119" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>206</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3862,38 +3885,38 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3962,7 +3985,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>77</v>
@@ -3972,7 +3995,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>77</v>
@@ -3982,10 +4005,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>

</xml_diff>